<commit_message>
add write sp signal to CU
</commit_message>
<xml_diff>
--- a/Design/Processor Design Analysis.xlsx
+++ b/Design/Processor Design Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material\3rd CMP\First term\Computer arch\Project\MIPS-Microprocessor-Design\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E382DA9E-2808-4D4D-8E7D-9E278F6176CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E451BD5-2037-4350-84F9-26ACDD317127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="204">
   <si>
     <t>Category of Operations</t>
   </si>
@@ -637,6 +637,9 @@
   <si>
     <t>Src1 in design</t>
   </si>
+  <si>
+    <t>write_sp</t>
+  </si>
 </sst>
 </file>
 
@@ -790,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -891,6 +894,7 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1125,7 +1129,7 @@
   <dimension ref="A1:AI1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1249,7 @@
       <c r="AI2" s="3"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2"/>
@@ -1296,7 +1300,7 @@
       <c r="AI3" s="3"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -1345,7 +1349,7 @@
       <c r="AI4" s="3"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>17</v>
@@ -1397,7 +1401,7 @@
       <c r="AI6" s="3"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="2"/>
@@ -1431,7 +1435,7 @@
       <c r="AI7" s="3"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
         <v>23</v>
@@ -1463,7 +1467,7 @@
       <c r="AI8" s="3"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>24</v>
@@ -1495,7 +1499,7 @@
       <c r="AI9" s="3"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>25</v>
@@ -1527,7 +1531,7 @@
       <c r="AI10" s="3"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1579,7 +1583,7 @@
       <c r="AI12" s="3"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="41" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="2"/>
@@ -1613,7 +1617,7 @@
       <c r="AI13" s="3"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
         <v>33</v>
@@ -1645,7 +1649,7 @@
       <c r="AI14" s="3"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>34</v>
@@ -1677,7 +1681,7 @@
       <c r="AI15" s="3"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
         <v>35</v>
@@ -1709,7 +1713,7 @@
       <c r="AI16" s="3"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
         <v>36</v>
@@ -1741,7 +1745,7 @@
       <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
         <v>37</v>
@@ -1773,7 +1777,7 @@
       <c r="AI18" s="3"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
         <v>39</v>
@@ -1825,7 +1829,7 @@
       <c r="AI20" s="3"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="41" t="s">
         <v>41</v>
       </c>
       <c r="B21" s="2"/>
@@ -1860,7 +1864,7 @@
       <c r="AI21" s="3"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
         <v>44</v>
@@ -1893,7 +1897,7 @@
       <c r="AI22" s="3"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
         <v>45</v>
@@ -1926,7 +1930,7 @@
       <c r="AI23" s="3"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
         <v>47</v>
@@ -1959,7 +1963,7 @@
       <c r="AI24" s="3"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
         <v>48</v>
@@ -2021,7 +2025,7 @@
       <c r="AI26" s="3"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="41" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="2"/>
@@ -2060,7 +2064,7 @@
       <c r="AI27" s="3"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1" t="s">
         <v>52</v>
@@ -2097,7 +2101,7 @@
       <c r="AI28" s="3"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="2"/>
       <c r="C29" s="1" t="s">
         <v>53</v>
@@ -2134,7 +2138,7 @@
       <c r="AI29" s="3"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="2"/>
       <c r="C30" s="12" t="s">
         <v>54</v>
@@ -2171,7 +2175,7 @@
       <c r="AI30" s="3"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
         <v>55</v>
@@ -2208,7 +2212,7 @@
       <c r="AI31" s="3"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="2"/>
       <c r="C32" s="12" t="s">
         <v>56</v>
@@ -2249,7 +2253,7 @@
       <c r="AI32" s="3"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
@@ -2290,7 +2294,7 @@
       <c r="AI33" s="3"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="2"/>
       <c r="C34" s="12" t="s">
         <v>58</v>
@@ -2331,7 +2335,7 @@
       <c r="AI34" s="3"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1" t="s">
         <v>60</v>
@@ -2372,7 +2376,7 @@
       <c r="AI35" s="3"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="2"/>
       <c r="C36" s="12" t="s">
         <v>62</v>
@@ -2471,7 +2475,7 @@
       <c r="AI38" s="3"/>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="41" t="s">
         <v>64</v>
       </c>
       <c r="B39" s="2"/>
@@ -2516,7 +2520,7 @@
       <c r="AI39" s="3"/>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A40" s="41"/>
+      <c r="A40" s="42"/>
       <c r="B40" s="2"/>
       <c r="C40" s="1" t="s">
         <v>66</v>
@@ -38782,46 +38786,46 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="43" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="41"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -38995,12 +38999,12 @@
     </row>
     <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
     </row>
@@ -68436,10 +68440,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C378BDBA-608F-43ED-BF6C-14DDA805CFD5}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -68450,12 +68454,13 @@
     <col min="11" max="11" width="14.44140625" customWidth="1"/>
     <col min="12" max="12" width="12.5546875" customWidth="1"/>
     <col min="13" max="13" width="16.44140625" customWidth="1"/>
-    <col min="14" max="14" width="17.77734375" customWidth="1"/>
-    <col min="15" max="15" width="37.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.77734375" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" style="40" customWidth="1"/>
+    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="16" max="16" width="37.6640625" customWidth="1"/>
+    <col min="17" max="17" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="31"/>
       <c r="B1" s="31" t="s">
         <v>169</v>
@@ -68493,14 +68498,17 @@
       <c r="M1" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="N1" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="Q1" s="34" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>9</v>
       </c>
@@ -68540,14 +68548,17 @@
       <c r="M2" s="25">
         <v>0</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="N2" s="25">
+        <v>0</v>
+      </c>
+      <c r="P2" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="P2" s="39" t="s">
+      <c r="Q2" s="39" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>15</v>
       </c>
@@ -68587,8 +68598,11 @@
       <c r="M3" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>17</v>
       </c>
@@ -68628,8 +68642,11 @@
       <c r="M4" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
@@ -68643,8 +68660,9 @@
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
       <c r="M5" s="26"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N5" s="26"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>20</v>
       </c>
@@ -68684,8 +68702,11 @@
       <c r="M6" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N6" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>23</v>
       </c>
@@ -68725,8 +68746,11 @@
       <c r="M7" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N7" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>24</v>
       </c>
@@ -68766,9 +68790,12 @@
       <c r="M8" s="25">
         <v>0</v>
       </c>
-      <c r="N8" s="27"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N8" s="25">
+        <v>0</v>
+      </c>
+      <c r="O8" s="27"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>25</v>
       </c>
@@ -68808,11 +68835,14 @@
       <c r="M9" s="25">
         <v>0</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="25">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>27</v>
       </c>
@@ -68852,9 +68882,12 @@
       <c r="M10" s="25">
         <v>0</v>
       </c>
-      <c r="N10" s="27"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N10" s="25">
+        <v>0</v>
+      </c>
+      <c r="O10" s="27"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -68868,8 +68901,9 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N11" s="26"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>30</v>
       </c>
@@ -68909,11 +68943,14 @@
       <c r="M12" s="25">
         <v>0</v>
       </c>
-      <c r="N12" s="27" t="s">
+      <c r="N12" s="25">
+        <v>0</v>
+      </c>
+      <c r="O12" s="27" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>33</v>
       </c>
@@ -68953,8 +68990,11 @@
       <c r="M13" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N13" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>34</v>
       </c>
@@ -68994,8 +69034,11 @@
       <c r="M14" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N14" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>35</v>
       </c>
@@ -69035,8 +69078,11 @@
       <c r="M15" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>36</v>
       </c>
@@ -69076,8 +69122,11 @@
       <c r="M16" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>37</v>
       </c>
@@ -69117,8 +69166,11 @@
       <c r="M17" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N17" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>39</v>
       </c>
@@ -69158,8 +69210,11 @@
       <c r="M18" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N18" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -69173,8 +69228,9 @@
       <c r="K19" s="26"/>
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="26"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>42</v>
       </c>
@@ -69214,11 +69270,14 @@
       <c r="M20" s="25">
         <v>0</v>
       </c>
-      <c r="N20" s="27" t="s">
+      <c r="N20" s="25">
+        <v>1</v>
+      </c>
+      <c r="O20" s="27" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>44</v>
       </c>
@@ -69258,9 +69317,12 @@
       <c r="M21" s="25">
         <v>0</v>
       </c>
-      <c r="N21" s="27"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N21" s="25">
+        <v>1</v>
+      </c>
+      <c r="O21" s="27"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>45</v>
       </c>
@@ -69300,11 +69362,14 @@
       <c r="M22" s="25">
         <v>1</v>
       </c>
-      <c r="N22" s="27" t="s">
+      <c r="N22" s="25">
+        <v>0</v>
+      </c>
+      <c r="O22" s="27" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>47</v>
       </c>
@@ -69344,11 +69409,14 @@
       <c r="M23" s="25">
         <v>0</v>
       </c>
-      <c r="N23" s="27" t="s">
+      <c r="N23" s="25">
+        <v>0</v>
+      </c>
+      <c r="O23" s="27" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>48</v>
       </c>
@@ -69388,11 +69456,14 @@
       <c r="M24" s="25">
         <v>0</v>
       </c>
-      <c r="N24" s="27" t="s">
+      <c r="N24" s="25">
+        <v>0</v>
+      </c>
+      <c r="O24" s="27" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
@@ -69406,8 +69477,9 @@
       <c r="K25" s="26"/>
       <c r="L25" s="26"/>
       <c r="M25" s="26"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N25" s="26"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>50</v>
       </c>
@@ -69447,11 +69519,14 @@
       <c r="M26" s="25">
         <v>0</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" s="25">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
         <v>52</v>
       </c>
@@ -69491,11 +69566,14 @@
       <c r="M27" s="25">
         <v>0</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="25">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
         <v>53</v>
       </c>
@@ -69535,11 +69613,14 @@
       <c r="M28" s="25">
         <v>0</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N28" s="25">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>55</v>
       </c>
@@ -69579,11 +69660,14 @@
       <c r="M29" s="25">
         <v>0</v>
       </c>
-      <c r="N29" s="24" t="s">
+      <c r="N29" s="25">
+        <v>0</v>
+      </c>
+      <c r="O29" s="24" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>57</v>
       </c>
@@ -69623,11 +69707,14 @@
       <c r="M30" s="25">
         <v>0</v>
       </c>
-      <c r="N30" s="24" t="s">
+      <c r="N30" s="25">
+        <v>0</v>
+      </c>
+      <c r="O30" s="24" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>60</v>
       </c>
@@ -69667,8 +69754,11 @@
       <c r="M31" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N31" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -69682,8 +69772,9 @@
       <c r="K32" s="26"/>
       <c r="L32" s="26"/>
       <c r="M32" s="26"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="26"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
@@ -69697,8 +69788,9 @@
       <c r="K33" s="26"/>
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="26"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
         <v>65</v>
       </c>
@@ -69714,8 +69806,9 @@
       <c r="K34" s="25"/>
       <c r="L34" s="25"/>
       <c r="M34" s="25"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="25"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
         <v>66</v>
       </c>
@@ -69731,6 +69824,7 @@
       <c r="K35" s="25"/>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add RTI instruction in ISA
</commit_message>
<xml_diff>
--- a/Design/Processor Design Analysis.xlsx
+++ b/Design/Processor Design Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material\3rd CMP\First term\Computer arch\Project\MIPS-Microprocessor-Design\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engineering\Third_Year\CMP_2023\First_Term\Arch\project\MIPS-Microprocessor-Design\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B42987-23A5-426A-B7EB-A130B8450B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5B4789-EAE7-45E6-B848-019989AA11DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="236">
   <si>
     <t>Category of Operations</t>
   </si>
@@ -734,6 +734,9 @@
   <si>
     <t>int</t>
   </si>
+  <si>
+    <t>RTI</t>
+  </si>
 </sst>
 </file>
 
@@ -899,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -950,15 +953,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -972,7 +972,6 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -981,9 +980,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1000,7 +996,6 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1010,6 +1005,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1023,7 +1019,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1242,10 +1237,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI1010"/>
+  <dimension ref="A1:AI1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1257,7 +1252,7 @@
     <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="3.44140625" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="3.21875" style="30" customWidth="1"/>
+    <col min="8" max="8" width="3.21875" customWidth="1"/>
     <col min="10" max="10" width="3.21875" customWidth="1"/>
     <col min="12" max="12" width="3.6640625" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" customWidth="1"/>
@@ -1291,11 +1286,11 @@
         <v>3</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="36" t="s">
         <v>210</v>
       </c>
       <c r="J1" s="2"/>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="36" t="s">
         <v>211</v>
       </c>
       <c r="L1" s="2"/>
@@ -1365,7 +1360,7 @@
       <c r="AI2" s="3"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2"/>
@@ -1381,11 +1376,11 @@
         <v>9</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="4"/>
@@ -1416,7 +1411,7 @@
       <c r="AI3" s="3"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -1430,11 +1425,11 @@
         <v>14</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L4" s="4"/>
@@ -1465,7 +1460,7 @@
       <c r="AI4" s="3"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -1479,11 +1474,11 @@
         <v>16</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L5" s="4"/>
@@ -1517,7 +1512,7 @@
       <c r="AI6" s="3"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2"/>
@@ -1533,11 +1528,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="41" t="s">
+      <c r="K7" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L7" s="4"/>
@@ -1551,7 +1546,7 @@
       <c r="AI7" s="3"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
         <v>21</v>
@@ -1565,11 +1560,11 @@
         <v>14</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="41" t="s">
+      <c r="K8" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L8" s="4"/>
@@ -1583,7 +1578,7 @@
       <c r="AI8" s="3"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>22</v>
@@ -1597,11 +1592,11 @@
         <v>16</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L9" s="4"/>
@@ -1615,7 +1610,7 @@
       <c r="AI9" s="3"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>23</v>
@@ -1633,7 +1628,7 @@
         <v>11</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L10" s="4"/>
@@ -1647,7 +1642,7 @@
       <c r="AI10" s="3"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>25</v>
@@ -1665,7 +1660,7 @@
         <v>11</v>
       </c>
       <c r="J11" s="2"/>
-      <c r="K11" s="41" t="s">
+      <c r="K11" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="4"/>
@@ -1699,7 +1694,7 @@
       <c r="AI12" s="3"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="39" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="2"/>
@@ -1715,11 +1710,11 @@
         <v>9</v>
       </c>
       <c r="H13" s="9"/>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="9"/>
-      <c r="K13" s="41" t="s">
+      <c r="K13" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L13" s="4"/>
@@ -1733,7 +1728,7 @@
       <c r="AI13" s="3"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
         <v>31</v>
@@ -1747,11 +1742,11 @@
         <v>14</v>
       </c>
       <c r="H14" s="9"/>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J14" s="9"/>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="4"/>
@@ -1765,7 +1760,7 @@
       <c r="AI14" s="3"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1779,11 +1774,11 @@
         <v>16</v>
       </c>
       <c r="H15" s="9"/>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="9"/>
-      <c r="K15" s="41" t="s">
+      <c r="K15" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L15" s="4"/>
@@ -1797,7 +1792,7 @@
       <c r="AI15" s="3"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -1811,11 +1806,11 @@
         <v>24</v>
       </c>
       <c r="H16" s="9"/>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="9"/>
-      <c r="K16" s="41" t="s">
+      <c r="K16" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L16" s="4"/>
@@ -1829,7 +1824,7 @@
       <c r="AI16" s="3"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
         <v>34</v>
@@ -1843,11 +1838,11 @@
         <v>26</v>
       </c>
       <c r="H17" s="9"/>
-      <c r="I17" s="41" t="s">
+      <c r="I17" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="9"/>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L17" s="4"/>
@@ -1861,7 +1856,7 @@
       <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
         <v>35</v>
@@ -1875,11 +1870,11 @@
         <v>36</v>
       </c>
       <c r="H18" s="9"/>
-      <c r="I18" s="41" t="s">
+      <c r="I18" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="9"/>
-      <c r="K18" s="41" t="s">
+      <c r="K18" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L18" s="4"/>
@@ -1893,7 +1888,7 @@
       <c r="AI18" s="3"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
         <v>37</v>
@@ -1907,11 +1902,11 @@
         <v>38</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="41" t="s">
+      <c r="I19" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="9"/>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L19" s="4"/>
@@ -1945,7 +1940,7 @@
       <c r="AI20" s="3"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="39" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="2"/>
@@ -1961,11 +1956,11 @@
         <v>9</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J21" s="2"/>
-      <c r="K21" s="41" t="s">
+      <c r="K21" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L21" s="4"/>
@@ -1980,7 +1975,7 @@
       <c r="AI21" s="3"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
         <v>42</v>
@@ -1994,11 +1989,11 @@
         <v>14</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="43" t="s">
+      <c r="I22" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J22" s="2"/>
-      <c r="K22" s="41" t="s">
+      <c r="K22" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L22" s="4"/>
@@ -2013,7 +2008,7 @@
       <c r="AI22" s="3"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
         <v>43</v>
@@ -2027,11 +2022,11 @@
         <v>16</v>
       </c>
       <c r="H23" s="4"/>
-      <c r="I23" s="43" t="s">
+      <c r="I23" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J23" s="4"/>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L23" s="4"/>
@@ -2046,7 +2041,7 @@
       <c r="AI23" s="3"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
         <v>45</v>
@@ -2060,11 +2055,11 @@
         <v>24</v>
       </c>
       <c r="H24" s="9"/>
-      <c r="I24" s="41" t="s">
+      <c r="I24" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J24" s="9"/>
-      <c r="K24" s="41" t="s">
+      <c r="K24" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L24" s="4"/>
@@ -2079,7 +2074,7 @@
       <c r="AI24" s="3"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
         <v>46</v>
@@ -2093,11 +2088,11 @@
         <v>26</v>
       </c>
       <c r="H25" s="9"/>
-      <c r="I25" s="41" t="s">
+      <c r="I25" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J25" s="9"/>
-      <c r="K25" s="41" t="s">
+      <c r="K25" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L25" s="4"/>
@@ -2141,7 +2136,7 @@
       <c r="AI26" s="3"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="39" t="s">
         <v>47</v>
       </c>
       <c r="B27" s="2"/>
@@ -2157,11 +2152,11 @@
         <v>9</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="43" t="s">
+      <c r="I27" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J27" s="2"/>
-      <c r="K27" s="41" t="s">
+      <c r="K27" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L27" s="4"/>
@@ -2180,7 +2175,7 @@
       <c r="AI27" s="3"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1" t="s">
         <v>50</v>
@@ -2194,11 +2189,11 @@
         <v>14</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="43" t="s">
+      <c r="I28" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J28" s="2"/>
-      <c r="K28" s="41" t="s">
+      <c r="K28" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L28" s="4"/>
@@ -2217,7 +2212,7 @@
       <c r="AI28" s="3"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A29" s="45"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="2"/>
       <c r="C29" s="1" t="s">
         <v>51</v>
@@ -2231,11 +2226,11 @@
         <v>16</v>
       </c>
       <c r="H29" s="2"/>
-      <c r="I29" s="43" t="s">
+      <c r="I29" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J29" s="2"/>
-      <c r="K29" s="41" t="s">
+      <c r="K29" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L29" s="4"/>
@@ -2254,7 +2249,7 @@
       <c r="AI29" s="3"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="2"/>
       <c r="C30" s="12" t="s">
         <v>52</v>
@@ -2268,11 +2263,11 @@
         <v>24</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="I30" s="43" t="s">
+      <c r="I30" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J30" s="2"/>
-      <c r="K30" s="41" t="s">
+      <c r="K30" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L30" s="4"/>
@@ -2291,7 +2286,7 @@
       <c r="AI30" s="3"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
         <v>53</v>
@@ -2305,11 +2300,11 @@
         <v>26</v>
       </c>
       <c r="H31" s="2"/>
-      <c r="I31" s="43" t="s">
+      <c r="I31" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J31" s="2"/>
-      <c r="K31" s="41" t="s">
+      <c r="K31" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L31" s="4"/>
@@ -2328,7 +2323,7 @@
       <c r="AI31" s="3"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="2"/>
       <c r="C32" s="12" t="s">
         <v>54</v>
@@ -2342,11 +2337,11 @@
         <v>36</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="41" t="s">
+      <c r="I32" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J32" s="2"/>
-      <c r="K32" s="43" t="s">
+      <c r="K32" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L32" s="4"/>
@@ -2369,7 +2364,7 @@
       <c r="AI32" s="3"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
         <v>55</v>
@@ -2383,11 +2378,11 @@
         <v>38</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="43" t="s">
+      <c r="I33" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J33" s="2"/>
-      <c r="K33" s="41" t="s">
+      <c r="K33" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L33" s="4"/>
@@ -2410,7 +2405,7 @@
       <c r="AI33" s="3"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="2"/>
       <c r="C34" s="12" t="s">
         <v>56</v>
@@ -2424,11 +2419,11 @@
         <v>57</v>
       </c>
       <c r="H34" s="2"/>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J34" s="2"/>
-      <c r="K34" s="43" t="s">
+      <c r="K34" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L34" s="4"/>
@@ -2451,7 +2446,7 @@
       <c r="AI34" s="3"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1" t="s">
         <v>58</v>
@@ -2465,11 +2460,11 @@
         <v>59</v>
       </c>
       <c r="H35" s="2"/>
-      <c r="I35" s="43" t="s">
+      <c r="I35" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J35" s="2"/>
-      <c r="K35" s="41" t="s">
+      <c r="K35" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L35" s="4"/>
@@ -2492,7 +2487,7 @@
       <c r="AI35" s="3"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="45"/>
+      <c r="A36" s="40"/>
       <c r="B36" s="2"/>
       <c r="C36" s="12" t="s">
         <v>60</v>
@@ -2510,7 +2505,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="2"/>
-      <c r="K36" s="41" t="s">
+      <c r="K36" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L36" s="2"/>
@@ -2533,21 +2528,32 @@
       <c r="AI36" s="3"/>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="C37" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="5">
+        <v>100</v>
+      </c>
       <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="G37" s="5">
+        <v>1010</v>
+      </c>
       <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
+      <c r="I37" s="37" t="s">
+        <v>10</v>
+      </c>
       <c r="J37" s="2"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="K37" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" s="2"/>
+      <c r="M37" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
+      <c r="O37" s="1"/>
       <c r="P37" s="2"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
@@ -2591,40 +2597,24 @@
       <c r="AI38" s="3"/>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
-        <v>62</v>
-      </c>
+      <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E39" s="4"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="43" t="s">
-        <v>10</v>
-      </c>
+      <c r="I39" s="2"/>
       <c r="J39" s="2"/>
-      <c r="K39" s="43" t="s">
-        <v>11</v>
-      </c>
+      <c r="K39" s="9"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="M39" s="4"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="1"/>
+      <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
       <c r="AA39" s="3"/>
       <c r="AB39" s="3"/>
       <c r="AC39" s="3"/>
@@ -2636,12 +2626,14 @@
       <c r="AI39" s="3"/>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A40" s="45"/>
+      <c r="A40" s="39" t="s">
+        <v>62</v>
+      </c>
       <c r="B40" s="2"/>
       <c r="C40" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="D40" s="4"/>
       <c r="E40" s="6" t="s">
         <v>10</v>
       </c>
@@ -2650,11 +2642,11 @@
         <v>10</v>
       </c>
       <c r="H40" s="2"/>
-      <c r="I40" s="43" t="s">
+      <c r="I40" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J40" s="2"/>
-      <c r="K40" s="43" t="s">
+      <c r="K40" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L40" s="4"/>
@@ -2664,12 +2656,6 @@
       <c r="N40" s="2"/>
       <c r="O40" s="1"/>
       <c r="P40" s="2"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
@@ -2685,21 +2671,33 @@
       <c r="AI40" s="3"/>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="C41" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="E41" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="G41" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
+      <c r="I41" s="37" t="s">
+        <v>10</v>
+      </c>
       <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
+      <c r="K41" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="4"/>
+      <c r="M41" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
+      <c r="O41" s="1"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
@@ -2722,41 +2720,41 @@
       <c r="AI41" s="3"/>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
-      <c r="W42" s="1"/>
-      <c r="X42" s="1"/>
-      <c r="Y42" s="1"/>
-      <c r="Z42" s="1"/>
-      <c r="AA42" s="1"/>
-      <c r="AB42" s="1"/>
-      <c r="AC42" s="1"/>
-      <c r="AD42" s="1"/>
-      <c r="AE42" s="1"/>
-      <c r="AF42" s="1"/>
-      <c r="AG42" s="1"/>
-      <c r="AH42" s="1"/>
-      <c r="AI42" s="1"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="3"/>
+      <c r="AE42" s="3"/>
+      <c r="AF42" s="3"/>
+      <c r="AG42" s="3"/>
+      <c r="AH42" s="3"/>
+      <c r="AI42" s="3"/>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
@@ -8013,21 +8011,21 @@
       <c r="AI184" s="1"/>
     </row>
     <row r="185" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A185" s="1"/>
-      <c r="B185" s="2"/>
-      <c r="C185" s="1"/>
-      <c r="D185" s="2"/>
-      <c r="E185" s="1"/>
-      <c r="F185" s="2"/>
-      <c r="G185" s="1"/>
-      <c r="H185" s="2"/>
-      <c r="I185" s="1"/>
-      <c r="J185" s="2"/>
-      <c r="K185" s="1"/>
-      <c r="L185" s="2"/>
-      <c r="M185" s="1"/>
-      <c r="N185" s="2"/>
-      <c r="O185" s="1"/>
+      <c r="A185" s="3"/>
+      <c r="B185" s="3"/>
+      <c r="C185" s="3"/>
+      <c r="D185" s="3"/>
+      <c r="E185" s="3"/>
+      <c r="F185" s="3"/>
+      <c r="G185" s="3"/>
+      <c r="H185" s="3"/>
+      <c r="I185" s="3"/>
+      <c r="J185" s="3"/>
+      <c r="K185" s="3"/>
+      <c r="L185" s="3"/>
+      <c r="M185" s="3"/>
+      <c r="N185" s="3"/>
+      <c r="O185" s="3"/>
       <c r="P185" s="1"/>
       <c r="Q185" s="1"/>
       <c r="R185" s="1"/>
@@ -38574,9 +38572,46 @@
       <c r="AH1010" s="1"/>
       <c r="AI1010" s="1"/>
     </row>
+    <row r="1011" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1011" s="1"/>
+      <c r="B1011" s="2"/>
+      <c r="C1011" s="1"/>
+      <c r="D1011" s="2"/>
+      <c r="E1011" s="1"/>
+      <c r="F1011" s="2"/>
+      <c r="G1011" s="1"/>
+      <c r="H1011" s="2"/>
+      <c r="I1011" s="1"/>
+      <c r="J1011" s="2"/>
+      <c r="K1011" s="1"/>
+      <c r="L1011" s="2"/>
+      <c r="M1011" s="1"/>
+      <c r="N1011" s="2"/>
+      <c r="O1011" s="1"/>
+      <c r="P1011" s="1"/>
+      <c r="Q1011" s="1"/>
+      <c r="R1011" s="1"/>
+      <c r="S1011" s="1"/>
+      <c r="T1011" s="1"/>
+      <c r="U1011" s="1"/>
+      <c r="V1011" s="1"/>
+      <c r="W1011" s="1"/>
+      <c r="X1011" s="1"/>
+      <c r="Y1011" s="1"/>
+      <c r="Z1011" s="1"/>
+      <c r="AA1011" s="1"/>
+      <c r="AB1011" s="1"/>
+      <c r="AC1011" s="1"/>
+      <c r="AD1011" s="1"/>
+      <c r="AE1011" s="1"/>
+      <c r="AF1011" s="1"/>
+      <c r="AG1011" s="1"/>
+      <c r="AH1011" s="1"/>
+      <c r="AI1011" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A13:A19"/>
@@ -38640,7 +38675,7 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>146</v>
       </c>
       <c r="E4" s="16" t="s">
@@ -38654,7 +38689,7 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>147</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -38668,7 +38703,7 @@
       <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>148</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -38682,7 +38717,7 @@
       <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>149</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -38696,7 +38731,7 @@
       <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>150</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -38710,7 +38745,7 @@
       <c r="C9" s="3">
         <v>5</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>151</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -38724,7 +38759,7 @@
       <c r="C10" s="3">
         <v>6</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>152</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -38738,7 +38773,7 @@
       <c r="C11" s="3">
         <v>7</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>153</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -38752,7 +38787,7 @@
       <c r="C12" s="3">
         <v>8</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>154</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -38766,7 +38801,7 @@
       <c r="C13" s="3">
         <v>9</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>155</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -38780,7 +38815,7 @@
       <c r="C14" s="3">
         <v>10</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>156</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -38794,7 +38829,7 @@
       <c r="C15" s="3">
         <v>11</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>157</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -38808,7 +38843,7 @@
       <c r="C16" s="3">
         <v>12</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>158</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -38822,7 +38857,7 @@
       <c r="C17" s="3">
         <v>13</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="21" t="s">
         <v>159</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -38902,46 +38937,46 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="47" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="45"/>
+      <c r="I6" s="40"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -39115,12 +39150,12 @@
     </row>
     <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
     </row>
@@ -39272,7 +39307,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" s="20" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
@@ -39284,7 +39319,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" s="20" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
@@ -39350,23 +39385,23 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="25"/>
+      <c r="D26" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -68571,392 +68606,391 @@
     <col min="4" max="5" width="13.88671875" customWidth="1"/>
     <col min="11" max="11" width="14.44140625" customWidth="1"/>
     <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="16.44140625" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" style="40" customWidth="1"/>
+    <col min="13" max="14" width="16.44140625" customWidth="1"/>
     <col min="15" max="15" width="17.77734375" customWidth="1"/>
     <col min="16" max="16" width="37.6640625" customWidth="1"/>
     <col min="17" max="17" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="27" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="22">
         <v>0</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="22">
         <v>0</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="22">
         <v>0</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="22">
         <v>0</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="22">
         <v>0</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="22">
         <v>0</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="22">
         <v>0</v>
       </c>
-      <c r="J2" s="25">
+      <c r="J2" s="22">
         <v>0</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="22">
         <v>0</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="22">
         <v>0</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="22">
         <v>0</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="22">
         <v>0</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="P2" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="Q2" s="39" t="s">
+      <c r="Q2" s="34" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="22">
         <v>0</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="22">
         <v>0</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="22">
         <v>0</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="22">
         <v>0</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="22">
         <v>0</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="22">
         <v>0</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="22">
         <v>0</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="22">
         <v>0</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="22">
         <v>0</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="22">
         <v>0</v>
       </c>
-      <c r="M3" s="25">
+      <c r="M3" s="22">
         <v>0</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="22">
         <v>0</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <v>0</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="22">
         <v>0</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="22">
         <v>0</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="22">
         <v>0</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="22">
         <v>0</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="22">
         <v>0</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="22">
         <v>0</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="22">
         <v>0</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="22">
         <v>0</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="22">
         <v>0</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="22">
         <v>0</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <v>1</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <v>1</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>0</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <v>0</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <v>0</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="22">
         <v>0</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="22">
         <v>0</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="22">
         <v>0</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="22">
         <v>0</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="22">
         <v>0</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="22">
         <v>0</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="22">
         <v>1</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <v>1</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="22">
         <v>0</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="22">
         <v>0</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="22">
         <v>0</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="22">
         <v>0</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="22">
         <v>0</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="22">
         <v>0</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="22">
         <v>0</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="22">
         <v>0</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="22">
         <v>0</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="22">
         <v>1</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="22">
         <v>1</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>0</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="22">
         <v>0</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="22">
         <v>0</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="22">
         <v>0</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="22">
         <v>0</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="22">
         <v>0</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="22">
         <v>0</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="22">
         <v>0</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="22">
         <v>0</v>
       </c>
-      <c r="O8" s="27"/>
+      <c r="O8" s="24"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="22">
         <v>0</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="22">
         <v>1</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <v>0</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="22">
         <v>0</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="22">
         <v>0</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="22">
         <v>1</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="22">
         <v>1</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="22">
         <v>0</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="22">
         <v>0</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="22">
         <v>0</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="22">
         <v>0</v>
       </c>
-      <c r="N9" s="25">
+      <c r="N9" s="22">
         <v>0</v>
       </c>
-      <c r="O9" s="49" t="s">
+      <c r="O9" s="38" t="s">
         <v>194</v>
       </c>
       <c r="P9" t="s">
@@ -68964,683 +68998,683 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="22">
         <v>0</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <v>0</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
         <v>1</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="22">
         <v>0</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="22">
         <v>0</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="22">
         <v>1</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="22">
         <v>0</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="22">
         <v>1</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="22">
         <v>0</v>
       </c>
-      <c r="L10" s="25">
+      <c r="L10" s="22">
         <v>0</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="22">
         <v>0</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="22">
         <v>0</v>
       </c>
-      <c r="O10" s="27"/>
+      <c r="O10" s="24"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="22">
         <v>0</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="22">
         <v>1</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="22">
         <v>1</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="22">
         <v>0</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="22">
         <v>0</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="22">
         <v>0</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="22">
         <v>0</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="22">
         <v>0</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="22">
         <v>0</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="22">
         <v>0</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="22">
         <v>0</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12" s="22">
         <v>0</v>
       </c>
-      <c r="O12" s="27" t="s">
+      <c r="O12" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="22">
         <v>0</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="22">
         <v>1</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="22">
         <v>1</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="22">
         <v>0</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="22">
         <v>0</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="22">
         <v>0</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="22">
         <v>0</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="22">
         <v>0</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="22">
         <v>0</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="22">
         <v>0</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="22">
         <v>0</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="22">
         <v>0</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <v>1</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
         <v>1</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="22">
         <v>0</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="22">
         <v>0</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="22">
         <v>0</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="22">
         <v>0</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="22">
         <v>0</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="22">
         <v>0</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="22">
         <v>0</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="22">
         <v>0</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="22">
         <v>0</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="22">
         <v>1</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="22">
         <v>1</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="22">
         <v>0</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="22">
         <v>0</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="22">
         <v>0</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="22">
         <v>0</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="22">
         <v>0</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="22">
         <v>0</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15" s="22">
         <v>0</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="22">
         <v>0</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="22">
         <v>0</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="22">
         <v>1</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
         <v>1</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="22">
         <v>0</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="22">
         <v>0</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="22">
         <v>0</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="22">
         <v>0</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="22">
         <v>0</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="22">
         <v>0</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="22">
         <v>0</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="22">
         <v>0</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="22">
         <v>0</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="22">
         <v>1</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="22">
         <v>1</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="22">
         <v>0</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="22">
         <v>0</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="22">
         <v>0</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="22">
         <v>0</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="22">
         <v>0</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="22">
         <v>0</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="22">
         <v>0</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="22">
         <v>0</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="22">
         <v>0</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="22">
         <v>1</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
         <v>1</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="22">
         <v>0</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="22">
         <v>0</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="22">
         <v>0</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="22">
         <v>0</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="22">
         <v>0</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="22">
         <v>0</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="22">
         <v>0</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="22">
         <v>0</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="22">
         <v>0</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <v>1</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="22">
         <v>0</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="22">
         <v>0</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="22">
         <v>1</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="22">
         <v>0</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="22">
         <v>0</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="22">
         <v>0</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="22">
         <v>1</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20" s="22">
         <v>1</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="22">
         <v>0</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20" s="22">
         <v>1</v>
       </c>
-      <c r="O20" s="27" t="s">
+      <c r="O20" s="24" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="22">
         <v>0</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="22">
         <v>0</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="22">
         <v>1</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="22">
         <v>1</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="22">
         <v>0</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="22">
         <v>0</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="22">
         <v>0</v>
       </c>
-      <c r="J21" s="25">
+      <c r="J21" s="22">
         <v>0</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21" s="22">
         <v>1</v>
       </c>
-      <c r="L21" s="25">
+      <c r="L21" s="22">
         <v>0</v>
       </c>
-      <c r="M21" s="25">
+      <c r="M21" s="22">
         <v>0</v>
       </c>
-      <c r="N21" s="25">
+      <c r="N21" s="22">
         <v>1</v>
       </c>
-      <c r="O21" s="27"/>
+      <c r="O21" s="24"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="22">
         <v>0</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="22">
         <v>0</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="22">
         <v>1</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="22">
         <v>1</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="22">
         <v>0</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="22">
         <v>0</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="22">
         <v>0</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22" s="22">
         <v>0</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22" s="22">
         <v>0</v>
       </c>
-      <c r="L22" s="25">
+      <c r="L22" s="22">
         <v>0</v>
       </c>
-      <c r="M22" s="25">
+      <c r="M22" s="22">
         <v>1</v>
       </c>
-      <c r="N22" s="25">
+      <c r="N22" s="22">
         <v>0</v>
       </c>
-      <c r="O22" s="27" t="s">
+      <c r="O22" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23" s="22">
         <v>0</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="22">
         <v>1</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="22">
         <v>1</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="22">
         <v>1</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="22">
         <v>0</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="22">
         <v>0</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I23" s="22">
         <v>0</v>
       </c>
-      <c r="J23" s="25">
+      <c r="J23" s="22">
         <v>0</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="22">
         <v>0</v>
       </c>
-      <c r="L23" s="25">
+      <c r="L23" s="22">
         <v>0</v>
       </c>
-      <c r="M23" s="25">
+      <c r="M23" s="22">
         <v>0</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N23" s="22">
         <v>0</v>
       </c>
-      <c r="O23" s="27" t="s">
+      <c r="O23" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="22">
         <v>0</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <v>1</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="22">
         <v>0</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="22">
         <v>0</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="22">
         <v>1</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="22">
         <v>0</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24" s="22">
         <v>0</v>
       </c>
-      <c r="J24" s="25">
+      <c r="J24" s="22">
         <v>0</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="22">
         <v>0</v>
       </c>
-      <c r="L24" s="25">
+      <c r="L24" s="22">
         <v>0</v>
       </c>
-      <c r="M24" s="25">
+      <c r="M24" s="22">
         <v>0</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="22">
         <v>0</v>
       </c>
-      <c r="O24" s="27" t="s">
+      <c r="O24" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="22">
         <v>1</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="22">
         <v>1</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="22">
         <v>0</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="22">
         <v>0</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="22">
         <v>0</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="22">
         <v>0</v>
       </c>
-      <c r="I26" s="25">
+      <c r="I26" s="22">
         <v>0</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26" s="22">
         <v>0</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="22">
         <v>0</v>
       </c>
-      <c r="L26" s="25">
+      <c r="L26" s="22">
         <v>0</v>
       </c>
-      <c r="M26" s="25">
+      <c r="M26" s="22">
         <v>0</v>
       </c>
-      <c r="N26" s="25">
+      <c r="N26" s="22">
         <v>0</v>
       </c>
       <c r="O26" t="s">
@@ -69648,46 +69682,46 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="22">
         <v>1</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="22">
         <v>1</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="22">
         <v>0</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="22">
         <v>0</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="22">
         <v>0</v>
       </c>
-      <c r="H27" s="25">
+      <c r="H27" s="22">
         <v>0</v>
       </c>
-      <c r="I27" s="25">
+      <c r="I27" s="22">
         <v>0</v>
       </c>
-      <c r="J27" s="25">
+      <c r="J27" s="22">
         <v>0</v>
       </c>
-      <c r="K27" s="25">
+      <c r="K27" s="22">
         <v>0</v>
       </c>
-      <c r="L27" s="25">
+      <c r="L27" s="22">
         <v>0</v>
       </c>
-      <c r="M27" s="25">
+      <c r="M27" s="22">
         <v>0</v>
       </c>
-      <c r="N27" s="25">
+      <c r="N27" s="22">
         <v>0</v>
       </c>
       <c r="O27" t="s">
@@ -69695,46 +69729,46 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="22">
         <v>1</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="22">
         <v>1</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="22">
         <v>0</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="22">
         <v>0</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="22">
         <v>0</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H28" s="22">
         <v>0</v>
       </c>
-      <c r="I28" s="25">
+      <c r="I28" s="22">
         <v>0</v>
       </c>
-      <c r="J28" s="25">
+      <c r="J28" s="22">
         <v>0</v>
       </c>
-      <c r="K28" s="25">
+      <c r="K28" s="22">
         <v>0</v>
       </c>
-      <c r="L28" s="25">
+      <c r="L28" s="22">
         <v>0</v>
       </c>
-      <c r="M28" s="25">
+      <c r="M28" s="22">
         <v>0</v>
       </c>
-      <c r="N28" s="25">
+      <c r="N28" s="22">
         <v>0</v>
       </c>
       <c r="O28" t="s">
@@ -69742,210 +69776,210 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="22">
         <v>1</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="22">
         <v>0</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="22">
         <v>0</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="22">
         <v>0</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="22">
         <v>0</v>
       </c>
-      <c r="H29" s="25">
+      <c r="H29" s="22">
         <v>0</v>
       </c>
-      <c r="I29" s="25">
+      <c r="I29" s="22">
         <v>0</v>
       </c>
-      <c r="J29" s="25">
+      <c r="J29" s="22">
         <v>0</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="22">
         <v>0</v>
       </c>
-      <c r="L29" s="25">
+      <c r="L29" s="22">
         <v>0</v>
       </c>
-      <c r="M29" s="25">
+      <c r="M29" s="22">
         <v>0</v>
       </c>
-      <c r="N29" s="25">
+      <c r="N29" s="22">
         <v>0</v>
       </c>
-      <c r="O29" s="24" t="s">
+      <c r="O29" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C30" s="25">
+      <c r="C30" s="22">
         <v>1</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="22">
         <v>0</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="22">
         <v>0</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="22">
         <v>0</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="22">
         <v>0</v>
       </c>
-      <c r="H30" s="25">
+      <c r="H30" s="22">
         <v>0</v>
       </c>
-      <c r="I30" s="25">
+      <c r="I30" s="22">
         <v>0</v>
       </c>
-      <c r="J30" s="25">
+      <c r="J30" s="22">
         <v>0</v>
       </c>
-      <c r="K30" s="25">
+      <c r="K30" s="22">
         <v>0</v>
       </c>
-      <c r="L30" s="25">
+      <c r="L30" s="22">
         <v>0</v>
       </c>
-      <c r="M30" s="25">
+      <c r="M30" s="22">
         <v>0</v>
       </c>
-      <c r="N30" s="25">
+      <c r="N30" s="22">
         <v>0</v>
       </c>
-      <c r="O30" s="24" t="s">
+      <c r="O30" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="22">
         <v>1</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="22">
         <v>0</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="22">
         <v>0</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="22">
         <v>0</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="22">
         <v>0</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="22">
         <v>0</v>
       </c>
-      <c r="I31" s="25">
+      <c r="I31" s="22">
         <v>0</v>
       </c>
-      <c r="J31" s="25">
+      <c r="J31" s="22">
         <v>0</v>
       </c>
-      <c r="K31" s="25">
+      <c r="K31" s="22">
         <v>0</v>
       </c>
-      <c r="L31" s="25">
+      <c r="L31" s="22">
         <v>0</v>
       </c>
-      <c r="M31" s="25">
+      <c r="M31" s="22">
         <v>0</v>
       </c>
-      <c r="N31" s="25">
+      <c r="N31" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -69956,215 +69990,215 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04234B7-E967-4FCA-8035-6E4532CB5BC2}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="22">
         <v>1</v>
       </c>
-      <c r="K15" s="25" t="s">
+      <c r="K15" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="L15" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="M15" s="25" t="s">
+      <c r="M15" s="22" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="25" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="25" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="25" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="25" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="25" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="25" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="25" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="25" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="25" t="s">
         <v>234</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the CU for interrupts
</commit_message>
<xml_diff>
--- a/Design/Processor Design Analysis.xlsx
+++ b/Design/Processor Design Analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material\3rd CMP\First term\Computer arch\Project\MIPS-Microprocessor-Design\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20102\Desktop\MIPS-Microprocessor-Design\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5EE32B-D6E6-4D47-B7D3-EE0E89FFC3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DD9BF0-0F92-4D2C-ADA0-1422783C7728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="243">
   <si>
     <t>Category of Operations</t>
   </si>
@@ -929,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -980,15 +980,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1002,7 +999,6 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1011,9 +1007,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1030,7 +1023,6 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1041,10 +1033,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1056,9 +1047,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1294,7 +1282,7 @@
     <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="3.44140625" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="3.21875" style="30" customWidth="1"/>
+    <col min="8" max="8" width="3.21875" customWidth="1"/>
     <col min="10" max="10" width="3.21875" customWidth="1"/>
     <col min="12" max="12" width="3.6640625" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" customWidth="1"/>
@@ -1328,11 +1316,11 @@
         <v>3</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="36" t="s">
         <v>210</v>
       </c>
       <c r="J1" s="2"/>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="36" t="s">
         <v>211</v>
       </c>
       <c r="L1" s="2"/>
@@ -1402,7 +1390,7 @@
       <c r="AI2" s="3"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="40" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2"/>
@@ -1418,11 +1406,11 @@
         <v>9</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="4"/>
@@ -1453,7 +1441,7 @@
       <c r="AI3" s="3"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -1467,11 +1455,11 @@
         <v>14</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L4" s="4"/>
@@ -1502,7 +1490,7 @@
       <c r="AI4" s="3"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -1516,11 +1504,11 @@
         <v>16</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L5" s="4"/>
@@ -1554,7 +1542,7 @@
       <c r="AI6" s="3"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2"/>
@@ -1570,11 +1558,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="41" t="s">
+      <c r="K7" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L7" s="4"/>
@@ -1588,7 +1576,7 @@
       <c r="AI7" s="3"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
         <v>21</v>
@@ -1602,11 +1590,11 @@
         <v>14</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="41" t="s">
+      <c r="K8" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L8" s="4"/>
@@ -1620,7 +1608,7 @@
       <c r="AI8" s="3"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>22</v>
@@ -1634,11 +1622,11 @@
         <v>16</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L9" s="4"/>
@@ -1652,7 +1640,7 @@
       <c r="AI9" s="3"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>23</v>
@@ -1670,7 +1658,7 @@
         <v>11</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L10" s="4"/>
@@ -1684,7 +1672,7 @@
       <c r="AI10" s="3"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>25</v>
@@ -1702,7 +1690,7 @@
         <v>11</v>
       </c>
       <c r="J11" s="2"/>
-      <c r="K11" s="41" t="s">
+      <c r="K11" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="4"/>
@@ -1736,7 +1724,7 @@
       <c r="AI12" s="3"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="40" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="2"/>
@@ -1752,11 +1740,11 @@
         <v>9</v>
       </c>
       <c r="H13" s="9"/>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="9"/>
-      <c r="K13" s="41" t="s">
+      <c r="K13" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L13" s="4"/>
@@ -1770,7 +1758,7 @@
       <c r="AI13" s="3"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
         <v>31</v>
@@ -1784,11 +1772,11 @@
         <v>14</v>
       </c>
       <c r="H14" s="9"/>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J14" s="9"/>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="4"/>
@@ -1802,7 +1790,7 @@
       <c r="AI14" s="3"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1816,11 +1804,11 @@
         <v>16</v>
       </c>
       <c r="H15" s="9"/>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="9"/>
-      <c r="K15" s="41" t="s">
+      <c r="K15" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L15" s="4"/>
@@ -1834,7 +1822,7 @@
       <c r="AI15" s="3"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -1848,11 +1836,11 @@
         <v>24</v>
       </c>
       <c r="H16" s="9"/>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="9"/>
-      <c r="K16" s="41" t="s">
+      <c r="K16" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L16" s="4"/>
@@ -1866,7 +1854,7 @@
       <c r="AI16" s="3"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
         <v>34</v>
@@ -1880,11 +1868,11 @@
         <v>26</v>
       </c>
       <c r="H17" s="9"/>
-      <c r="I17" s="41" t="s">
+      <c r="I17" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="9"/>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L17" s="4"/>
@@ -1898,7 +1886,7 @@
       <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
         <v>35</v>
@@ -1912,11 +1900,11 @@
         <v>36</v>
       </c>
       <c r="H18" s="9"/>
-      <c r="I18" s="41" t="s">
+      <c r="I18" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="9"/>
-      <c r="K18" s="41" t="s">
+      <c r="K18" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L18" s="4"/>
@@ -1930,7 +1918,7 @@
       <c r="AI18" s="3"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
         <v>37</v>
@@ -1944,11 +1932,11 @@
         <v>38</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="41" t="s">
+      <c r="I19" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="9"/>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L19" s="4"/>
@@ -1982,7 +1970,7 @@
       <c r="AI20" s="3"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="40" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="2"/>
@@ -1998,11 +1986,11 @@
         <v>9</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J21" s="2"/>
-      <c r="K21" s="41" t="s">
+      <c r="K21" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L21" s="4"/>
@@ -2017,7 +2005,7 @@
       <c r="AI21" s="3"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
         <v>42</v>
@@ -2031,11 +2019,11 @@
         <v>14</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="43" t="s">
+      <c r="I22" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J22" s="2"/>
-      <c r="K22" s="41" t="s">
+      <c r="K22" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L22" s="4"/>
@@ -2050,7 +2038,7 @@
       <c r="AI22" s="3"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
         <v>43</v>
@@ -2064,11 +2052,11 @@
         <v>16</v>
       </c>
       <c r="H23" s="4"/>
-      <c r="I23" s="43" t="s">
+      <c r="I23" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J23" s="4"/>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L23" s="4"/>
@@ -2083,7 +2071,7 @@
       <c r="AI23" s="3"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
         <v>45</v>
@@ -2097,11 +2085,11 @@
         <v>24</v>
       </c>
       <c r="H24" s="9"/>
-      <c r="I24" s="41" t="s">
+      <c r="I24" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J24" s="9"/>
-      <c r="K24" s="41" t="s">
+      <c r="K24" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L24" s="4"/>
@@ -2116,7 +2104,7 @@
       <c r="AI24" s="3"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
         <v>46</v>
@@ -2130,11 +2118,11 @@
         <v>26</v>
       </c>
       <c r="H25" s="9"/>
-      <c r="I25" s="41" t="s">
+      <c r="I25" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J25" s="9"/>
-      <c r="K25" s="41" t="s">
+      <c r="K25" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L25" s="4"/>
@@ -2178,7 +2166,7 @@
       <c r="AI26" s="3"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="40" t="s">
         <v>47</v>
       </c>
       <c r="B27" s="2"/>
@@ -2194,11 +2182,11 @@
         <v>9</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="43" t="s">
+      <c r="I27" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J27" s="2"/>
-      <c r="K27" s="41" t="s">
+      <c r="K27" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L27" s="4"/>
@@ -2217,7 +2205,7 @@
       <c r="AI27" s="3"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1" t="s">
         <v>50</v>
@@ -2231,11 +2219,11 @@
         <v>14</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="43" t="s">
+      <c r="I28" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J28" s="2"/>
-      <c r="K28" s="41" t="s">
+      <c r="K28" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L28" s="4"/>
@@ -2254,7 +2242,7 @@
       <c r="AI28" s="3"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="2"/>
       <c r="C29" s="1" t="s">
         <v>51</v>
@@ -2268,11 +2256,11 @@
         <v>16</v>
       </c>
       <c r="H29" s="2"/>
-      <c r="I29" s="43" t="s">
+      <c r="I29" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J29" s="2"/>
-      <c r="K29" s="41" t="s">
+      <c r="K29" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L29" s="4"/>
@@ -2291,7 +2279,7 @@
       <c r="AI29" s="3"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="2"/>
       <c r="C30" s="12" t="s">
         <v>52</v>
@@ -2305,11 +2293,11 @@
         <v>24</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="I30" s="43" t="s">
+      <c r="I30" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J30" s="2"/>
-      <c r="K30" s="41" t="s">
+      <c r="K30" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L30" s="4"/>
@@ -2328,7 +2316,7 @@
       <c r="AI30" s="3"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
         <v>53</v>
@@ -2342,11 +2330,11 @@
         <v>26</v>
       </c>
       <c r="H31" s="2"/>
-      <c r="I31" s="43" t="s">
+      <c r="I31" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J31" s="2"/>
-      <c r="K31" s="41" t="s">
+      <c r="K31" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L31" s="4"/>
@@ -2365,7 +2353,7 @@
       <c r="AI31" s="3"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="2"/>
       <c r="C32" s="12" t="s">
         <v>54</v>
@@ -2379,11 +2367,11 @@
         <v>36</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="41" t="s">
+      <c r="I32" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J32" s="2"/>
-      <c r="K32" s="43" t="s">
+      <c r="K32" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L32" s="4"/>
@@ -2406,7 +2394,7 @@
       <c r="AI32" s="3"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
         <v>55</v>
@@ -2420,11 +2408,11 @@
         <v>38</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="43" t="s">
+      <c r="I33" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J33" s="2"/>
-      <c r="K33" s="41" t="s">
+      <c r="K33" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L33" s="4"/>
@@ -2447,7 +2435,7 @@
       <c r="AI33" s="3"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="2"/>
       <c r="C34" s="12" t="s">
         <v>56</v>
@@ -2461,11 +2449,11 @@
         <v>57</v>
       </c>
       <c r="H34" s="2"/>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J34" s="2"/>
-      <c r="K34" s="43" t="s">
+      <c r="K34" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L34" s="4"/>
@@ -2488,7 +2476,7 @@
       <c r="AI34" s="3"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1" t="s">
         <v>58</v>
@@ -2502,11 +2490,11 @@
         <v>59</v>
       </c>
       <c r="H35" s="2"/>
-      <c r="I35" s="43" t="s">
+      <c r="I35" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J35" s="2"/>
-      <c r="K35" s="41" t="s">
+      <c r="K35" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L35" s="4"/>
@@ -2529,7 +2517,7 @@
       <c r="AI35" s="3"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="2"/>
       <c r="C36" s="12" t="s">
         <v>60</v>
@@ -2547,7 +2535,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="2"/>
-      <c r="K36" s="41" t="s">
+      <c r="K36" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L36" s="2"/>
@@ -2569,9 +2557,9 @@
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
     </row>
-    <row r="37" spans="1:35" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
-      <c r="C37" s="52" t="s">
+      <c r="C37" s="39" t="s">
         <v>241</v>
       </c>
       <c r="D37" s="2"/>
@@ -2587,7 +2575,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="2"/>
-      <c r="K37" s="41" t="s">
+      <c r="K37" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L37" s="2"/>
@@ -2595,7 +2583,7 @@
         <v>12</v>
       </c>
       <c r="N37" s="2"/>
-      <c r="O37" s="45"/>
+      <c r="O37" s="1"/>
       <c r="P37" s="2"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
@@ -2668,7 +2656,7 @@
       <c r="AI39" s="3"/>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B40" s="2"/>
@@ -2684,11 +2672,11 @@
         <v>10</v>
       </c>
       <c r="H40" s="2"/>
-      <c r="I40" s="43" t="s">
+      <c r="I40" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J40" s="2"/>
-      <c r="K40" s="43" t="s">
+      <c r="K40" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L40" s="4"/>
@@ -2713,7 +2701,7 @@
       <c r="AI40" s="3"/>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
+      <c r="A41" s="41"/>
       <c r="B41" s="2"/>
       <c r="C41" s="1" t="s">
         <v>64</v>
@@ -2727,11 +2715,11 @@
         <v>10</v>
       </c>
       <c r="H41" s="2"/>
-      <c r="I41" s="43" t="s">
+      <c r="I41" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J41" s="2"/>
-      <c r="K41" s="43" t="s">
+      <c r="K41" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L41" s="4"/>
@@ -38717,7 +38705,7 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>146</v>
       </c>
       <c r="E4" s="16" t="s">
@@ -38731,7 +38719,7 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>147</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -38745,7 +38733,7 @@
       <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>148</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -38759,7 +38747,7 @@
       <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>149</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -38773,7 +38761,7 @@
       <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>150</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -38787,7 +38775,7 @@
       <c r="C9" s="3">
         <v>5</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>151</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -38801,7 +38789,7 @@
       <c r="C10" s="3">
         <v>6</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>152</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -38815,7 +38803,7 @@
       <c r="C11" s="3">
         <v>7</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>153</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -38829,7 +38817,7 @@
       <c r="C12" s="3">
         <v>8</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>154</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -38843,7 +38831,7 @@
       <c r="C13" s="3">
         <v>9</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>155</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -38857,7 +38845,7 @@
       <c r="C14" s="3">
         <v>10</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>156</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -38871,7 +38859,7 @@
       <c r="C15" s="3">
         <v>11</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>157</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -38885,7 +38873,7 @@
       <c r="C16" s="3">
         <v>12</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>158</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -38899,7 +38887,7 @@
       <c r="C17" s="3">
         <v>13</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="21" t="s">
         <v>159</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -38979,46 +38967,46 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="50" t="s">
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="48"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -39192,12 +39180,12 @@
     </row>
     <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
     </row>
@@ -39349,7 +39337,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" s="20" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
@@ -39361,7 +39349,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" s="20" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
@@ -39427,23 +39415,23 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="25"/>
+      <c r="D26" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -68637,8 +68625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C378BDBA-608F-43ED-BF6C-14DDA805CFD5}">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -68648,493 +68636,491 @@
     <col min="4" max="5" width="13.88671875" customWidth="1"/>
     <col min="11" max="11" width="14.44140625" customWidth="1"/>
     <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="16.44140625" customWidth="1"/>
-    <col min="14" max="17" width="16.44140625" style="46" customWidth="1"/>
-    <col min="18" max="18" width="16.44140625" style="40" customWidth="1"/>
+    <col min="13" max="18" width="16.44140625" customWidth="1"/>
     <col min="19" max="19" width="17.77734375" customWidth="1"/>
     <col min="20" max="20" width="37.6640625" customWidth="1"/>
     <col min="21" max="21" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="U1" s="27" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="22">
         <v>0</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="22">
         <v>0</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="22">
         <v>0</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="22">
         <v>0</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="22">
         <v>0</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="22">
         <v>0</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="22">
         <v>0</v>
       </c>
-      <c r="J2" s="25">
+      <c r="J2" s="22">
         <v>0</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="22">
         <v>0</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="22">
         <v>0</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="22">
         <v>0</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="22">
         <v>0</v>
       </c>
-      <c r="O2" s="25">
+      <c r="O2" s="22">
         <v>0</v>
       </c>
-      <c r="P2" s="25">
+      <c r="P2" s="22">
         <v>0</v>
       </c>
-      <c r="Q2" s="25">
+      <c r="Q2" s="22">
         <v>0</v>
       </c>
-      <c r="R2" s="25">
+      <c r="R2" s="22">
         <v>0</v>
       </c>
-      <c r="T2" s="35" t="s">
+      <c r="T2" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="U2" s="39" t="s">
+      <c r="U2" s="34" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="22">
         <v>0</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="22">
         <v>0</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="22">
         <v>0</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="22">
         <v>0</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="22">
         <v>0</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="22">
         <v>0</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="22">
         <v>0</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="22">
         <v>0</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="22">
         <v>0</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="22">
         <v>0</v>
       </c>
-      <c r="M3" s="25">
+      <c r="M3" s="22">
         <v>0</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3" s="22">
         <v>0</v>
       </c>
-      <c r="O3" s="25">
+      <c r="O3" s="22">
         <v>0</v>
       </c>
-      <c r="P3" s="25">
+      <c r="P3" s="22">
         <v>0</v>
       </c>
-      <c r="Q3" s="25">
+      <c r="Q3" s="22">
         <v>0</v>
       </c>
-      <c r="R3" s="25">
+      <c r="R3" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="22">
         <v>0</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <v>0</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="22">
         <v>0</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="22">
         <v>0</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="22">
         <v>0</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="22">
         <v>0</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="22">
         <v>0</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="22">
         <v>0</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="22">
         <v>0</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="22">
         <v>0</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="22">
         <v>0</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="22">
         <v>0</v>
       </c>
-      <c r="O4" s="25">
+      <c r="O4" s="22">
         <v>0</v>
       </c>
-      <c r="P4" s="25">
+      <c r="P4" s="22">
         <v>0</v>
       </c>
-      <c r="Q4" s="25">
+      <c r="Q4" s="22">
         <v>0</v>
       </c>
-      <c r="R4" s="25">
+      <c r="R4" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="22">
         <v>0</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <v>1</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <v>1</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>0</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <v>0</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <v>0</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="22">
         <v>0</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="22">
         <v>0</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="22">
         <v>0</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="22">
         <v>0</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="22">
         <v>0</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="22">
         <v>0</v>
       </c>
-      <c r="O6" s="25">
+      <c r="O6" s="22">
         <v>0</v>
       </c>
-      <c r="P6" s="25">
+      <c r="P6" s="22">
         <v>0</v>
       </c>
-      <c r="Q6" s="25">
+      <c r="Q6" s="22">
         <v>0</v>
       </c>
-      <c r="R6" s="25">
+      <c r="R6" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="22">
         <v>0</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="22">
         <v>1</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <v>1</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="22">
         <v>0</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="22">
         <v>0</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="22">
         <v>0</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="22">
         <v>0</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="22">
         <v>0</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="22">
         <v>0</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="22">
         <v>0</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="22">
         <v>0</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="22">
         <v>0</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="22">
         <v>0</v>
       </c>
-      <c r="P7" s="25">
+      <c r="P7" s="22">
         <v>0</v>
       </c>
-      <c r="Q7" s="25">
+      <c r="Q7" s="22">
         <v>0</v>
       </c>
-      <c r="R7" s="25">
+      <c r="R7" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="22">
         <v>0</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="22">
         <v>1</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="22">
         <v>1</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>0</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="22">
         <v>0</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="22">
         <v>0</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="22">
         <v>0</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="22">
         <v>0</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="22">
         <v>0</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="22">
         <v>0</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="22">
         <v>0</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="22">
         <v>0</v>
       </c>
-      <c r="O8" s="25">
+      <c r="O8" s="22">
         <v>0</v>
       </c>
-      <c r="P8" s="25">
+      <c r="P8" s="22">
         <v>0</v>
       </c>
-      <c r="Q8" s="25">
+      <c r="Q8" s="22">
         <v>0</v>
       </c>
-      <c r="R8" s="25">
+      <c r="R8" s="22">
         <v>0</v>
       </c>
-      <c r="S8" s="27"/>
+      <c r="S8" s="24"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="22">
         <v>0</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="22">
         <v>1</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <v>0</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="22">
         <v>0</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="22">
         <v>0</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="22">
         <v>1</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="22">
         <v>1</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="22">
         <v>0</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="22">
         <v>0</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="22">
         <v>0</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="22">
         <v>0</v>
       </c>
-      <c r="N9" s="25">
+      <c r="N9" s="22">
         <v>0</v>
       </c>
-      <c r="O9" s="25">
+      <c r="O9" s="22">
         <v>0</v>
       </c>
-      <c r="P9" s="25">
+      <c r="P9" s="22">
         <v>0</v>
       </c>
-      <c r="Q9" s="25">
+      <c r="Q9" s="22">
         <v>0</v>
       </c>
-      <c r="R9" s="25">
+      <c r="R9" s="22">
         <v>0</v>
       </c>
-      <c r="S9" s="44" t="s">
+      <c r="S9" s="38" t="s">
         <v>194</v>
       </c>
       <c r="T9" t="s">
@@ -69142,863 +69128,863 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="22">
         <v>0</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <v>0</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
         <v>1</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="22">
         <v>0</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="22">
         <v>0</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="22">
         <v>1</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="22">
         <v>0</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="22">
         <v>1</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="22">
         <v>0</v>
       </c>
-      <c r="L10" s="25">
+      <c r="L10" s="22">
         <v>0</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="22">
         <v>0</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="22">
         <v>0</v>
       </c>
-      <c r="O10" s="25">
+      <c r="O10" s="22">
         <v>0</v>
       </c>
-      <c r="P10" s="25">
+      <c r="P10" s="22">
         <v>0</v>
       </c>
-      <c r="Q10" s="25">
+      <c r="Q10" s="22">
         <v>0</v>
       </c>
-      <c r="R10" s="25">
+      <c r="R10" s="22">
         <v>0</v>
       </c>
-      <c r="S10" s="27"/>
+      <c r="S10" s="24"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="22">
         <v>0</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="22">
         <v>1</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="22">
         <v>1</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="22">
         <v>0</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="22">
         <v>0</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="22">
         <v>0</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="22">
         <v>0</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="22">
         <v>0</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="22">
         <v>0</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="22">
         <v>0</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="22">
         <v>0</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12" s="22">
         <v>0</v>
       </c>
-      <c r="O12" s="25">
+      <c r="O12" s="22">
         <v>0</v>
       </c>
-      <c r="P12" s="25">
+      <c r="P12" s="22">
         <v>0</v>
       </c>
-      <c r="Q12" s="25">
+      <c r="Q12" s="22">
         <v>0</v>
       </c>
-      <c r="R12" s="25">
+      <c r="R12" s="22">
         <v>0</v>
       </c>
-      <c r="S12" s="27" t="s">
+      <c r="S12" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="22">
         <v>0</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="22">
         <v>1</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="22">
         <v>1</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="22">
         <v>0</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="22">
         <v>0</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="22">
         <v>0</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="22">
         <v>0</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="22">
         <v>0</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="22">
         <v>0</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="22">
         <v>0</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="22">
         <v>0</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="22">
         <v>0</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="22">
         <v>0</v>
       </c>
-      <c r="P13" s="25">
+      <c r="P13" s="22">
         <v>0</v>
       </c>
-      <c r="Q13" s="25">
+      <c r="Q13" s="22">
         <v>0</v>
       </c>
-      <c r="R13" s="25">
+      <c r="R13" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="22">
         <v>0</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <v>1</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
         <v>1</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="22">
         <v>0</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="22">
         <v>0</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="22">
         <v>0</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="22">
         <v>0</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="22">
         <v>0</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="22">
         <v>0</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="22">
         <v>0</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="22">
         <v>0</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="22">
         <v>0</v>
       </c>
-      <c r="O14" s="25">
+      <c r="O14" s="22">
         <v>0</v>
       </c>
-      <c r="P14" s="25">
+      <c r="P14" s="22">
         <v>0</v>
       </c>
-      <c r="Q14" s="25">
+      <c r="Q14" s="22">
         <v>0</v>
       </c>
-      <c r="R14" s="25">
+      <c r="R14" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="22">
         <v>0</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="22">
         <v>1</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="22">
         <v>1</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="22">
         <v>0</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="22">
         <v>0</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="22">
         <v>0</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="22">
         <v>0</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="22">
         <v>0</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="22">
         <v>0</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15" s="22">
         <v>0</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="22">
         <v>0</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="22">
         <v>0</v>
       </c>
-      <c r="O15" s="25">
+      <c r="O15" s="22">
         <v>0</v>
       </c>
-      <c r="P15" s="25">
+      <c r="P15" s="22">
         <v>0</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q15" s="22">
         <v>0</v>
       </c>
-      <c r="R15" s="25">
+      <c r="R15" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="22">
         <v>0</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="22">
         <v>1</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
         <v>1</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="22">
         <v>0</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="22">
         <v>0</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="22">
         <v>0</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="22">
         <v>0</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="22">
         <v>0</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="22">
         <v>0</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="22">
         <v>0</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="22">
         <v>0</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="22">
         <v>0</v>
       </c>
-      <c r="O16" s="25">
+      <c r="O16" s="22">
         <v>0</v>
       </c>
-      <c r="P16" s="25">
+      <c r="P16" s="22">
         <v>0</v>
       </c>
-      <c r="Q16" s="25">
+      <c r="Q16" s="22">
         <v>0</v>
       </c>
-      <c r="R16" s="25">
+      <c r="R16" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="22">
         <v>0</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="22">
         <v>1</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="22">
         <v>1</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="22">
         <v>0</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="22">
         <v>0</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="22">
         <v>0</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="22">
         <v>0</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="22">
         <v>0</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="22">
         <v>0</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="22">
         <v>0</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="22">
         <v>0</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="22">
         <v>0</v>
       </c>
-      <c r="O17" s="25">
+      <c r="O17" s="22">
         <v>0</v>
       </c>
-      <c r="P17" s="25">
+      <c r="P17" s="22">
         <v>0</v>
       </c>
-      <c r="Q17" s="25">
+      <c r="Q17" s="22">
         <v>0</v>
       </c>
-      <c r="R17" s="25">
+      <c r="R17" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="22">
         <v>0</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="22">
         <v>1</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
         <v>1</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="22">
         <v>0</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="22">
         <v>0</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="22">
         <v>0</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="22">
         <v>0</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="22">
         <v>0</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="22">
         <v>0</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="22">
         <v>0</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="22">
         <v>0</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="22">
         <v>0</v>
       </c>
-      <c r="O18" s="25">
+      <c r="O18" s="22">
         <v>0</v>
       </c>
-      <c r="P18" s="25">
+      <c r="P18" s="22">
         <v>0</v>
       </c>
-      <c r="Q18" s="25">
+      <c r="Q18" s="22">
         <v>0</v>
       </c>
-      <c r="R18" s="25">
+      <c r="R18" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="22">
         <v>0</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <v>1</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="22">
         <v>0</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="22">
         <v>0</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="22">
         <v>1</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="22">
         <v>0</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="22">
         <v>0</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="22">
         <v>0</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="22">
         <v>1</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20" s="22">
         <v>1</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="22">
         <v>0</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20" s="22">
         <v>1</v>
       </c>
-      <c r="O20" s="25">
+      <c r="O20" s="22">
         <v>0</v>
       </c>
-      <c r="P20" s="25">
+      <c r="P20" s="22">
         <v>0</v>
       </c>
-      <c r="Q20" s="25">
+      <c r="Q20" s="22">
         <v>0</v>
       </c>
-      <c r="R20" s="25">
+      <c r="R20" s="22">
         <v>1</v>
       </c>
-      <c r="S20" s="27" t="s">
+      <c r="S20" s="24" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="22">
         <v>0</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="22">
         <v>0</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="22">
         <v>1</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="22">
         <v>1</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="22">
         <v>0</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="22">
         <v>0</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="22">
         <v>0</v>
       </c>
-      <c r="J21" s="25">
+      <c r="J21" s="22">
         <v>0</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21" s="22">
         <v>1</v>
       </c>
-      <c r="L21" s="25">
+      <c r="L21" s="22">
         <v>0</v>
       </c>
-      <c r="M21" s="25">
+      <c r="M21" s="22">
         <v>0</v>
       </c>
-      <c r="N21" s="25">
+      <c r="N21" s="22">
         <v>1</v>
       </c>
-      <c r="O21" s="25">
+      <c r="O21" s="22">
         <v>0</v>
       </c>
-      <c r="P21" s="25">
+      <c r="P21" s="22">
         <v>0</v>
       </c>
-      <c r="Q21" s="25">
+      <c r="Q21" s="22">
         <v>0</v>
       </c>
-      <c r="R21" s="25">
+      <c r="R21" s="22">
         <v>1</v>
       </c>
-      <c r="S21" s="27"/>
+      <c r="S21" s="24"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="22">
         <v>0</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="22">
         <v>0</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="22">
         <v>1</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="22">
         <v>1</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="22">
         <v>0</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="22">
         <v>0</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="22">
         <v>0</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22" s="22">
         <v>0</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22" s="22">
         <v>0</v>
       </c>
-      <c r="L22" s="25">
+      <c r="L22" s="22">
         <v>0</v>
       </c>
-      <c r="M22" s="25">
+      <c r="M22" s="22">
         <v>1</v>
       </c>
-      <c r="N22" s="25">
+      <c r="N22" s="22">
         <v>0</v>
       </c>
-      <c r="O22" s="25">
+      <c r="O22" s="22">
         <v>0</v>
       </c>
-      <c r="P22" s="25">
+      <c r="P22" s="22">
         <v>0</v>
       </c>
-      <c r="Q22" s="25">
+      <c r="Q22" s="22">
         <v>0</v>
       </c>
-      <c r="R22" s="25">
+      <c r="R22" s="22">
         <v>0</v>
       </c>
-      <c r="S22" s="27" t="s">
+      <c r="S22" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23" s="22">
         <v>0</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="22">
         <v>1</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="22">
         <v>1</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="22">
         <v>1</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="22">
         <v>0</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="22">
         <v>0</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I23" s="22">
         <v>0</v>
       </c>
-      <c r="J23" s="25">
+      <c r="J23" s="22">
         <v>0</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="22">
         <v>0</v>
       </c>
-      <c r="L23" s="25">
+      <c r="L23" s="22">
         <v>0</v>
       </c>
-      <c r="M23" s="25">
+      <c r="M23" s="22">
         <v>0</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N23" s="22">
         <v>0</v>
       </c>
-      <c r="O23" s="25">
+      <c r="O23" s="22">
         <v>0</v>
       </c>
-      <c r="P23" s="25">
+      <c r="P23" s="22">
         <v>0</v>
       </c>
-      <c r="Q23" s="25">
+      <c r="Q23" s="22">
         <v>0</v>
       </c>
-      <c r="R23" s="25">
+      <c r="R23" s="22">
         <v>0</v>
       </c>
-      <c r="S23" s="27" t="s">
+      <c r="S23" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="22">
         <v>0</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <v>1</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="22">
         <v>0</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="22">
         <v>0</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="22">
         <v>1</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="22">
         <v>0</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24" s="22">
         <v>0</v>
       </c>
-      <c r="J24" s="25">
+      <c r="J24" s="22">
         <v>0</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="22">
         <v>0</v>
       </c>
-      <c r="L24" s="25">
+      <c r="L24" s="22">
         <v>0</v>
       </c>
-      <c r="M24" s="25">
+      <c r="M24" s="22">
         <v>0</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="22">
         <v>0</v>
       </c>
-      <c r="O24" s="25">
+      <c r="O24" s="22">
         <v>0</v>
       </c>
-      <c r="P24" s="25">
+      <c r="P24" s="22">
         <v>0</v>
       </c>
-      <c r="Q24" s="25">
+      <c r="Q24" s="22">
         <v>0</v>
       </c>
-      <c r="R24" s="25">
+      <c r="R24" s="22">
         <v>0</v>
       </c>
-      <c r="S24" s="27" t="s">
+      <c r="S24" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="22">
         <v>1</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="22">
         <v>1</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="22">
         <v>0</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="22">
         <v>0</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="22">
         <v>0</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="22">
         <v>0</v>
       </c>
-      <c r="I26" s="25">
+      <c r="I26" s="22">
         <v>0</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26" s="22">
         <v>0</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="22">
         <v>0</v>
       </c>
-      <c r="L26" s="25">
+      <c r="L26" s="22">
         <v>0</v>
       </c>
-      <c r="M26" s="25">
+      <c r="M26" s="22">
         <v>0</v>
       </c>
-      <c r="N26" s="25">
+      <c r="N26" s="22">
         <v>0</v>
       </c>
-      <c r="O26" s="25">
+      <c r="O26" s="22">
         <v>0</v>
       </c>
-      <c r="P26" s="25">
+      <c r="P26" s="22">
         <v>0</v>
       </c>
-      <c r="Q26" s="25">
+      <c r="Q26" s="22">
         <v>0</v>
       </c>
-      <c r="R26" s="25" t="s">
+      <c r="R26" s="22" t="s">
         <v>236</v>
       </c>
       <c r="S26" t="s">
@@ -70006,58 +69992,58 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="22">
         <v>1</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="22">
         <v>1</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="22">
         <v>0</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="22">
         <v>0</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="22">
         <v>0</v>
       </c>
-      <c r="H27" s="25">
+      <c r="H27" s="22">
         <v>0</v>
       </c>
-      <c r="I27" s="25">
+      <c r="I27" s="22">
         <v>0</v>
       </c>
-      <c r="J27" s="25">
+      <c r="J27" s="22">
         <v>0</v>
       </c>
-      <c r="K27" s="25">
+      <c r="K27" s="22">
         <v>0</v>
       </c>
-      <c r="L27" s="25">
+      <c r="L27" s="22">
         <v>0</v>
       </c>
-      <c r="M27" s="25">
+      <c r="M27" s="22">
         <v>0</v>
       </c>
-      <c r="N27" s="25">
+      <c r="N27" s="22">
         <v>0</v>
       </c>
-      <c r="O27" s="25">
+      <c r="O27" s="22">
         <v>0</v>
       </c>
-      <c r="P27" s="25">
+      <c r="P27" s="22">
         <v>0</v>
       </c>
-      <c r="Q27" s="25">
+      <c r="Q27" s="22">
         <v>0</v>
       </c>
-      <c r="R27" s="25" t="s">
+      <c r="R27" s="22" t="s">
         <v>237</v>
       </c>
       <c r="S27" t="s">
@@ -70065,58 +70051,58 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="22">
         <v>1</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="22">
         <v>1</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="22">
         <v>0</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="22">
         <v>0</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="22">
         <v>0</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H28" s="22">
         <v>0</v>
       </c>
-      <c r="I28" s="25">
+      <c r="I28" s="22">
         <v>0</v>
       </c>
-      <c r="J28" s="25">
+      <c r="J28" s="22">
         <v>0</v>
       </c>
-      <c r="K28" s="25">
+      <c r="K28" s="22">
         <v>0</v>
       </c>
-      <c r="L28" s="25">
+      <c r="L28" s="22">
         <v>0</v>
       </c>
-      <c r="M28" s="25">
+      <c r="M28" s="22">
         <v>0</v>
       </c>
-      <c r="N28" s="25">
+      <c r="N28" s="22">
         <v>0</v>
       </c>
-      <c r="O28" s="25">
+      <c r="O28" s="22">
         <v>0</v>
       </c>
-      <c r="P28" s="25">
+      <c r="P28" s="22">
         <v>0</v>
       </c>
-      <c r="Q28" s="25">
+      <c r="Q28" s="22">
         <v>0</v>
       </c>
-      <c r="R28" s="25" t="s">
+      <c r="R28" s="22" t="s">
         <v>238</v>
       </c>
       <c r="S28" t="s">
@@ -70124,318 +70110,344 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="22">
         <v>1</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="22">
         <v>0</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="22">
         <v>0</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="22">
         <v>0</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="22">
         <v>0</v>
       </c>
-      <c r="H29" s="25">
+      <c r="H29" s="22">
         <v>0</v>
       </c>
-      <c r="I29" s="25">
+      <c r="I29" s="22">
         <v>0</v>
       </c>
-      <c r="J29" s="25">
+      <c r="J29" s="22">
         <v>0</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="22">
         <v>0</v>
       </c>
-      <c r="L29" s="25">
+      <c r="L29" s="22">
         <v>0</v>
       </c>
-      <c r="M29" s="25">
+      <c r="M29" s="22">
         <v>0</v>
       </c>
-      <c r="N29" s="25">
+      <c r="N29" s="22">
         <v>0</v>
       </c>
-      <c r="O29" s="25">
+      <c r="O29" s="22">
         <v>0</v>
       </c>
-      <c r="P29" s="25">
+      <c r="P29" s="22">
         <v>0</v>
       </c>
-      <c r="Q29" s="25">
+      <c r="Q29" s="22">
         <v>0</v>
       </c>
-      <c r="R29" s="25" t="s">
+      <c r="R29" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="S29" s="24" t="s">
+      <c r="S29" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C30" s="25">
+      <c r="C30" s="22">
         <v>0</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="22">
         <v>0</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="22">
         <v>0</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="22">
         <v>0</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="22">
         <v>0</v>
       </c>
-      <c r="H30" s="25">
+      <c r="H30" s="22">
         <v>0</v>
       </c>
-      <c r="I30" s="25">
+      <c r="I30" s="22">
         <v>0</v>
       </c>
-      <c r="J30" s="25">
+      <c r="J30" s="22">
         <v>0</v>
       </c>
-      <c r="K30" s="25">
+      <c r="K30" s="22">
         <v>0</v>
       </c>
-      <c r="L30" s="25">
+      <c r="L30" s="22">
         <v>0</v>
       </c>
-      <c r="M30" s="25">
+      <c r="M30" s="22">
         <v>0</v>
       </c>
-      <c r="N30" s="25">
+      <c r="N30" s="22">
         <v>0</v>
       </c>
-      <c r="O30" s="25">
+      <c r="O30" s="22">
         <v>0</v>
       </c>
-      <c r="P30" s="25">
+      <c r="P30" s="22">
         <v>0</v>
       </c>
-      <c r="Q30" s="25">
+      <c r="Q30" s="22">
         <v>1</v>
       </c>
-      <c r="R30" s="25">
+      <c r="R30" s="22">
         <v>0</v>
       </c>
-      <c r="S30" s="24" t="s">
+      <c r="S30" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="C31" s="25">
+      <c r="B31" s="33">
         <v>0</v>
       </c>
-      <c r="D31" s="25">
+      <c r="C31" s="22">
+        <v>1</v>
+      </c>
+      <c r="D31" s="22">
         <v>0</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="22">
         <v>0</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="22">
         <v>0</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="22">
         <v>0</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="22">
         <v>0</v>
       </c>
-      <c r="I31" s="25">
+      <c r="I31" s="22">
         <v>0</v>
       </c>
-      <c r="J31" s="25">
+      <c r="J31" s="22">
         <v>0</v>
       </c>
-      <c r="K31" s="25">
+      <c r="K31" s="22">
         <v>0</v>
       </c>
-      <c r="L31" s="25">
+      <c r="L31" s="22">
         <v>0</v>
       </c>
-      <c r="M31" s="25">
+      <c r="M31" s="22">
         <v>0</v>
       </c>
-      <c r="N31" s="25">
+      <c r="N31" s="22">
         <v>0</v>
       </c>
-      <c r="O31" s="25">
+      <c r="O31" s="22">
         <v>0</v>
       </c>
-      <c r="P31" s="25">
+      <c r="P31" s="22">
         <v>1</v>
       </c>
-      <c r="Q31" s="25">
+      <c r="Q31" s="22">
         <v>0</v>
       </c>
-      <c r="R31" s="25">
+      <c r="R31" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="C32" s="25">
+      <c r="B32" s="33">
         <v>0</v>
       </c>
-      <c r="D32" s="25">
+      <c r="C32" s="22">
+        <v>1</v>
+      </c>
+      <c r="D32" s="22">
         <v>0</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="22">
+        <v>1</v>
+      </c>
+      <c r="F32" s="22">
+        <v>1</v>
+      </c>
+      <c r="G32" s="22">
         <v>0</v>
       </c>
-      <c r="F32" s="25">
+      <c r="H32" s="22">
         <v>0</v>
       </c>
-      <c r="G32" s="25">
+      <c r="I32" s="22">
         <v>0</v>
       </c>
-      <c r="H32" s="25">
+      <c r="J32" s="22">
         <v>0</v>
       </c>
-      <c r="I32" s="25">
+      <c r="K32" s="22">
+        <v>1</v>
+      </c>
+      <c r="L32" s="22">
         <v>0</v>
       </c>
-      <c r="J32" s="25">
+      <c r="M32" s="22">
         <v>0</v>
       </c>
-      <c r="K32" s="25">
+      <c r="N32" s="22">
+        <v>1</v>
+      </c>
+      <c r="O32" s="22">
+        <v>1</v>
+      </c>
+      <c r="P32" s="22">
         <v>0</v>
       </c>
-      <c r="L32" s="25">
+      <c r="Q32" s="22">
         <v>0</v>
       </c>
-      <c r="M32" s="25">
+      <c r="R32" s="22">
         <v>0</v>
       </c>
-      <c r="N32" s="25">
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="22">
+        <v>100</v>
+      </c>
+      <c r="C36" s="22">
+        <v>1</v>
+      </c>
+      <c r="D36" s="22">
+        <v>1</v>
+      </c>
+      <c r="E36" s="22">
+        <v>1</v>
+      </c>
+      <c r="F36" s="22">
         <v>0</v>
       </c>
-      <c r="O32" s="25">
+      <c r="G36" s="22">
         <v>1</v>
       </c>
-      <c r="P32" s="25">
+      <c r="H36" s="22">
         <v>0</v>
       </c>
-      <c r="Q32" s="25">
+      <c r="I36" s="22">
         <v>0</v>
       </c>
-      <c r="R32" s="25">
+      <c r="J36" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="26"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="25"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="25"/>
+      <c r="K36" s="22">
+        <v>1</v>
+      </c>
+      <c r="L36" s="22">
+        <v>1</v>
+      </c>
+      <c r="M36" s="22">
+        <v>0</v>
+      </c>
+      <c r="N36" s="22">
+        <v>1</v>
+      </c>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -70453,214 +70465,214 @@
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="22">
         <v>1</v>
       </c>
-      <c r="K15" s="25" t="s">
+      <c r="K15" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="L15" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="M15" s="25" t="s">
+      <c r="M15" s="22" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="25" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="25" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="25" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="25" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="25" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="25" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="25" t="s">
         <v>234</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add shl,shr reg to cu
</commit_message>
<xml_diff>
--- a/Design/Processor Design Analysis.xlsx
+++ b/Design/Processor Design Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material\3rd CMP\First term\Computer arch\Project\MIPS-Microprocessor-Design\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ACAE99-7B30-4453-9B8E-6D68CEC52459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849D829E-2972-4256-8039-F17F32458074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="243">
   <si>
     <t>Category of Operations</t>
   </si>
@@ -681,12 +681,6 @@
     <t>or</t>
   </si>
   <si>
-    <t>shl</t>
-  </si>
-  <si>
-    <t>shr</t>
-  </si>
-  <si>
     <t>in</t>
   </si>
   <si>
@@ -748,6 +742,21 @@
   </si>
   <si>
     <t>001010</t>
+  </si>
+  <si>
+    <t>SHL Rsrc, Rdst</t>
+  </si>
+  <si>
+    <t>SHR Rsrc, Rdst</t>
+  </si>
+  <si>
+    <t>SHL Rsrc, IMM</t>
+  </si>
+  <si>
+    <t>shl imm</t>
+  </si>
+  <si>
+    <t>shr imm</t>
   </si>
 </sst>
 </file>
@@ -926,7 +935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1049,6 +1058,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1057,9 +1073,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1279,10 +1292,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI1011"/>
+  <dimension ref="A1:AI1013"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1402,7 +1415,7 @@
       <c r="AI2" s="3"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="51" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2"/>
@@ -1453,7 +1466,7 @@
       <c r="AI3" s="3"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -1502,7 +1515,7 @@
       <c r="AI4" s="3"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -1554,7 +1567,7 @@
       <c r="AI6" s="3"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="51" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2"/>
@@ -1588,7 +1601,7 @@
       <c r="AI7" s="3"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
         <v>21</v>
@@ -1620,7 +1633,7 @@
       <c r="AI8" s="3"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>22</v>
@@ -1652,7 +1665,7 @@
       <c r="AI9" s="3"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>23</v>
@@ -1684,7 +1697,7 @@
       <c r="AI10" s="3"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>25</v>
@@ -1736,7 +1749,7 @@
       <c r="AI12" s="3"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="51" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="2"/>
@@ -1770,7 +1783,7 @@
       <c r="AI13" s="3"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
         <v>31</v>
@@ -1802,7 +1815,7 @@
       <c r="AI14" s="3"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1834,7 +1847,7 @@
       <c r="AI15" s="3"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -1866,7 +1879,7 @@
       <c r="AI16" s="3"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
         <v>34</v>
@@ -1898,10 +1911,10 @@
       <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>238</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="8" t="s">
@@ -1930,10 +1943,10 @@
       <c r="AI18" s="3"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
-        <v>37</v>
+        <v>239</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="8" t="s">
@@ -1960,120 +1973,116 @@
       <c r="P19" s="2"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+    <row r="20" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="51"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="9"/>
+      <c r="G20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="41" t="s">
+        <v>30</v>
+      </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="41" t="s">
+        <v>44</v>
+      </c>
       <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
+      <c r="O20" s="48"/>
       <c r="P20" s="2"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
-        <v>39</v>
-      </c>
+    <row r="21" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="51"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="5" t="s">
-        <v>41</v>
+      <c r="C21" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="9"/>
       <c r="K21" s="41" t="s">
         <v>30</v>
       </c>
       <c r="L21" s="4"/>
-      <c r="M21" s="7" t="s">
-        <v>12</v>
+      <c r="M21" s="41" t="s">
+        <v>44</v>
       </c>
       <c r="N21" s="2"/>
-      <c r="O21" s="1"/>
+      <c r="O21" s="48"/>
       <c r="P21" s="2"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="43" t="s">
-        <v>10</v>
-      </c>
+      <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="41" t="s">
-        <v>30</v>
-      </c>
+      <c r="K22" s="9"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="M22" s="4"/>
       <c r="N22" s="2"/>
-      <c r="O22" s="1"/>
+      <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
+      <c r="A23" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="5" t="s">
         <v>41</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="H23" s="2"/>
       <c r="I23" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="J23" s="4"/>
+      <c r="J23" s="2"/>
       <c r="K23" s="41" t="s">
         <v>30</v>
       </c>
       <c r="L23" s="4"/>
-      <c r="M23" s="11" t="s">
-        <v>44</v>
+      <c r="M23" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="1"/>
@@ -2083,10 +2092,10 @@
       <c r="AI23" s="3"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="8" t="s">
@@ -2094,13 +2103,13 @@
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="2"/>
       <c r="K24" s="41" t="s">
         <v>30</v>
       </c>
@@ -2116,10 +2125,10 @@
       <c r="AI24" s="3"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
+      <c r="A25" s="52"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="8" t="s">
@@ -2127,77 +2136,79 @@
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="4"/>
       <c r="K25" s="41" t="s">
         <v>30</v>
       </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="7" t="s">
-        <v>12</v>
+      <c r="M25" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="1"/>
       <c r="P25" s="2"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
-      <c r="AA25" s="3"/>
-      <c r="AF25" s="3"/>
-      <c r="AG25" s="3"/>
-      <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="A26" s="52"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="9"/>
+      <c r="G26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="41" t="s">
+        <v>30</v>
+      </c>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="M26" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
+      <c r="O26" s="1"/>
       <c r="P26" s="2"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
-      <c r="AA26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
-        <v>47</v>
-      </c>
+      <c r="A27" s="52"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="J27" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="9"/>
       <c r="K27" s="41" t="s">
         <v>30</v>
       </c>
@@ -2217,33 +2228,21 @@
       <c r="AI27" s="3"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
+      <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="8" t="s">
-        <v>49</v>
-      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="43" t="s">
-        <v>10</v>
-      </c>
+      <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="41" t="s">
-        <v>30</v>
-      </c>
+      <c r="K28" s="9"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="M28" s="4"/>
       <c r="N28" s="2"/>
-      <c r="O28" s="1"/>
+      <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
@@ -2254,18 +2253,20 @@
       <c r="AI28" s="3"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
+      <c r="A29" s="51" t="s">
+        <v>47</v>
+      </c>
       <c r="B29" s="2"/>
       <c r="C29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="43" t="s">
@@ -2291,18 +2292,18 @@
       <c r="AI29" s="3"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
+      <c r="A30" s="52"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="12" t="s">
-        <v>52</v>
+      <c r="C30" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="11">
-        <v>100</v>
+      <c r="E30" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="43" t="s">
@@ -2328,10 +2329,10 @@
       <c r="AI30" s="3"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
+      <c r="A31" s="52"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="8" t="s">
@@ -2339,7 +2340,7 @@
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="43" t="s">
@@ -2365,10 +2366,10 @@
       <c r="AI31" s="3"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
+      <c r="A32" s="52"/>
       <c r="B32" s="2"/>
       <c r="C32" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="11">
@@ -2376,19 +2377,19 @@
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="41" t="s">
-        <v>20</v>
+      <c r="I32" s="43" t="s">
+        <v>10</v>
       </c>
       <c r="J32" s="2"/>
-      <c r="K32" s="43" t="s">
-        <v>11</v>
+      <c r="K32" s="41" t="s">
+        <v>30</v>
       </c>
       <c r="L32" s="4"/>
-      <c r="M32" s="11" t="s">
-        <v>44</v>
+      <c r="M32" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="1"/>
@@ -2396,20 +2397,16 @@
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
       <c r="AA32" s="3"/>
-      <c r="AB32" s="3"/>
-      <c r="AC32" s="3"/>
-      <c r="AD32" s="3"/>
-      <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
       <c r="AH32" s="3"/>
       <c r="AI32" s="3"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
+      <c r="A33" s="52"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="8" t="s">
@@ -2417,7 +2414,7 @@
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="43" t="s">
@@ -2437,20 +2434,16 @@
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
       <c r="AA33" s="3"/>
-      <c r="AB33" s="3"/>
-      <c r="AC33" s="3"/>
-      <c r="AD33" s="3"/>
-      <c r="AE33" s="3"/>
       <c r="AF33" s="3"/>
       <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
+      <c r="A34" s="52"/>
       <c r="B34" s="2"/>
       <c r="C34" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="11">
@@ -2458,7 +2451,7 @@
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="5" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="41" t="s">
@@ -2488,10 +2481,10 @@
       <c r="AI34" s="3"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
+      <c r="A35" s="52"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="8" t="s">
@@ -2499,15 +2492,15 @@
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="5" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="43" t="s">
         <v>10</v>
       </c>
       <c r="J35" s="2"/>
-      <c r="K35" s="53" t="s">
-        <v>11</v>
+      <c r="K35" s="41" t="s">
+        <v>30</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="7" t="s">
@@ -2529,30 +2522,30 @@
       <c r="AI35" s="3"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
+      <c r="A36" s="52"/>
       <c r="B36" s="2"/>
       <c r="C36" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="11">
+        <v>100</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H36" s="2"/>
-      <c r="I36" s="10" t="s">
+      <c r="I36" s="41" t="s">
         <v>20</v>
       </c>
       <c r="J36" s="2"/>
-      <c r="K36" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="L36" s="2"/>
-      <c r="M36" s="7" t="s">
-        <v>12</v>
+      <c r="K36" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="4"/>
+      <c r="M36" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="1"/>
@@ -2569,33 +2562,34 @@
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
     </row>
-    <row r="37" spans="1:35" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A37" s="52"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="47" t="s">
-        <v>238</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="5" t="s">
+      <c r="C37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="8" t="s">
         <v>49</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="5" t="s">
-        <v>239</v>
+        <v>59</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="43" t="s">
         <v>10</v>
       </c>
       <c r="J37" s="2"/>
-      <c r="K37" s="53" t="s">
+      <c r="K37" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="L37" s="2"/>
+      <c r="L37" s="4"/>
       <c r="M37" s="7" t="s">
         <v>12</v>
       </c>
       <c r="N37" s="2"/>
-      <c r="O37" s="45"/>
+      <c r="O37" s="1"/>
       <c r="P37" s="2"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
@@ -2610,21 +2604,33 @@
       <c r="AI37" s="3"/>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
+      <c r="A38" s="52"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="C38" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="G38" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="I38" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="J38" s="2"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
+      <c r="K38" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="2"/>
+      <c r="M38" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
+      <c r="O38" s="1"/>
       <c r="P38" s="2"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
@@ -2638,22 +2644,33 @@
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
+    <row r="39" spans="1:35" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="C39" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="G39" s="5" t="s">
+        <v>237</v>
+      </c>
       <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="I39" s="43" t="s">
+        <v>10</v>
+      </c>
       <c r="J39" s="2"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="K39" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" s="2"/>
+      <c r="M39" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
+      <c r="O39" s="45"/>
       <c r="P39" s="2"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
@@ -2668,40 +2685,24 @@
       <c r="AI39" s="3"/>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
-        <v>62</v>
-      </c>
+      <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="C40" s="2"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E40" s="4"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="43" t="s">
-        <v>10</v>
-      </c>
+      <c r="I40" s="2"/>
       <c r="J40" s="2"/>
-      <c r="K40" s="43" t="s">
-        <v>11</v>
-      </c>
+      <c r="K40" s="9"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="M40" s="4"/>
       <c r="N40" s="2"/>
-      <c r="O40" s="1"/>
+      <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
-      <c r="Y40" s="3"/>
-      <c r="Z40" s="3"/>
       <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
@@ -2713,44 +2714,24 @@
       <c r="AI40" s="3"/>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="G41" s="2"/>
       <c r="H41" s="2"/>
-      <c r="I41" s="43" t="s">
-        <v>10</v>
-      </c>
+      <c r="I41" s="2"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="43" t="s">
-        <v>11</v>
-      </c>
+      <c r="K41" s="9"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="M41" s="4"/>
       <c r="N41" s="2"/>
-      <c r="O41" s="1"/>
+      <c r="O41" s="2"/>
       <c r="P41" s="2"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
       <c r="AB41" s="3"/>
       <c r="AC41" s="3"/>
@@ -2762,28 +2743,36 @@
       <c r="AI41" s="3"/>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
+      <c r="A42" s="51" t="s">
+        <v>62</v>
+      </c>
       <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="C42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="G42" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="I42" s="43" t="s">
+        <v>10</v>
+      </c>
       <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
+      <c r="K42" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="4"/>
+      <c r="M42" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
+      <c r="O42" s="1"/>
       <c r="P42" s="2"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
@@ -2799,78 +2788,90 @@
       <c r="AI42" s="3"/>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-      <c r="Y43" s="1"/>
-      <c r="Z43" s="1"/>
-      <c r="AA43" s="1"/>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="1"/>
-      <c r="AD43" s="1"/>
-      <c r="AE43" s="1"/>
-      <c r="AF43" s="1"/>
-      <c r="AG43" s="1"/>
-      <c r="AH43" s="1"/>
-      <c r="AI43" s="1"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="J43" s="2"/>
+      <c r="K43" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" s="4"/>
+      <c r="M43" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N43" s="2"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Y43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="3"/>
+      <c r="AC43" s="3"/>
+      <c r="AD43" s="3"/>
+      <c r="AE43" s="3"/>
+      <c r="AF43" s="3"/>
+      <c r="AG43" s="3"/>
+      <c r="AH43" s="3"/>
+      <c r="AI43" s="3"/>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
-      <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
-      <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
-      <c r="Z44" s="1"/>
-      <c r="AA44" s="1"/>
-      <c r="AB44" s="1"/>
-      <c r="AC44" s="1"/>
-      <c r="AD44" s="1"/>
-      <c r="AE44" s="1"/>
-      <c r="AF44" s="1"/>
-      <c r="AG44" s="1"/>
-      <c r="AH44" s="1"/>
-      <c r="AI44" s="1"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3"/>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3"/>
+      <c r="AC44" s="3"/>
+      <c r="AD44" s="3"/>
+      <c r="AE44" s="3"/>
+      <c r="AF44" s="3"/>
+      <c r="AG44" s="3"/>
+      <c r="AH44" s="3"/>
+      <c r="AI44" s="3"/>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
@@ -8090,21 +8091,21 @@
       <c r="AI185" s="1"/>
     </row>
     <row r="186" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A186" s="1"/>
-      <c r="B186" s="2"/>
-      <c r="C186" s="1"/>
-      <c r="D186" s="2"/>
-      <c r="E186" s="1"/>
-      <c r="F186" s="2"/>
-      <c r="G186" s="1"/>
-      <c r="H186" s="2"/>
-      <c r="I186" s="1"/>
-      <c r="J186" s="2"/>
-      <c r="K186" s="1"/>
-      <c r="L186" s="2"/>
-      <c r="M186" s="1"/>
-      <c r="N186" s="2"/>
-      <c r="O186" s="1"/>
+      <c r="A186" s="3"/>
+      <c r="B186" s="3"/>
+      <c r="C186" s="3"/>
+      <c r="D186" s="3"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="3"/>
+      <c r="G186" s="3"/>
+      <c r="H186" s="3"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="3"/>
+      <c r="K186" s="3"/>
+      <c r="L186" s="3"/>
+      <c r="M186" s="3"/>
+      <c r="N186" s="3"/>
+      <c r="O186" s="3"/>
       <c r="P186" s="1"/>
       <c r="Q186" s="1"/>
       <c r="R186" s="1"/>
@@ -8127,21 +8128,21 @@
       <c r="AI186" s="1"/>
     </row>
     <row r="187" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A187" s="1"/>
-      <c r="B187" s="2"/>
-      <c r="C187" s="1"/>
-      <c r="D187" s="2"/>
-      <c r="E187" s="1"/>
-      <c r="F187" s="2"/>
-      <c r="G187" s="1"/>
-      <c r="H187" s="2"/>
-      <c r="I187" s="1"/>
-      <c r="J187" s="2"/>
-      <c r="K187" s="1"/>
-      <c r="L187" s="2"/>
-      <c r="M187" s="1"/>
-      <c r="N187" s="2"/>
-      <c r="O187" s="1"/>
+      <c r="A187" s="3"/>
+      <c r="B187" s="3"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="3"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="3"/>
+      <c r="G187" s="3"/>
+      <c r="H187" s="3"/>
+      <c r="I187" s="3"/>
+      <c r="J187" s="3"/>
+      <c r="K187" s="3"/>
+      <c r="L187" s="3"/>
+      <c r="M187" s="3"/>
+      <c r="N187" s="3"/>
+      <c r="O187" s="3"/>
       <c r="P187" s="1"/>
       <c r="Q187" s="1"/>
       <c r="R187" s="1"/>
@@ -38651,14 +38652,88 @@
       <c r="AH1011" s="1"/>
       <c r="AI1011" s="1"/>
     </row>
+    <row r="1012" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1012" s="1"/>
+      <c r="B1012" s="2"/>
+      <c r="C1012" s="1"/>
+      <c r="D1012" s="2"/>
+      <c r="E1012" s="1"/>
+      <c r="F1012" s="2"/>
+      <c r="G1012" s="1"/>
+      <c r="H1012" s="2"/>
+      <c r="I1012" s="1"/>
+      <c r="J1012" s="2"/>
+      <c r="K1012" s="1"/>
+      <c r="L1012" s="2"/>
+      <c r="M1012" s="1"/>
+      <c r="N1012" s="2"/>
+      <c r="O1012" s="1"/>
+      <c r="P1012" s="1"/>
+      <c r="Q1012" s="1"/>
+      <c r="R1012" s="1"/>
+      <c r="S1012" s="1"/>
+      <c r="T1012" s="1"/>
+      <c r="U1012" s="1"/>
+      <c r="V1012" s="1"/>
+      <c r="W1012" s="1"/>
+      <c r="X1012" s="1"/>
+      <c r="Y1012" s="1"/>
+      <c r="Z1012" s="1"/>
+      <c r="AA1012" s="1"/>
+      <c r="AB1012" s="1"/>
+      <c r="AC1012" s="1"/>
+      <c r="AD1012" s="1"/>
+      <c r="AE1012" s="1"/>
+      <c r="AF1012" s="1"/>
+      <c r="AG1012" s="1"/>
+      <c r="AH1012" s="1"/>
+      <c r="AI1012" s="1"/>
+    </row>
+    <row r="1013" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1013" s="1"/>
+      <c r="B1013" s="2"/>
+      <c r="C1013" s="1"/>
+      <c r="D1013" s="2"/>
+      <c r="E1013" s="1"/>
+      <c r="F1013" s="2"/>
+      <c r="G1013" s="1"/>
+      <c r="H1013" s="2"/>
+      <c r="I1013" s="1"/>
+      <c r="J1013" s="2"/>
+      <c r="K1013" s="1"/>
+      <c r="L1013" s="2"/>
+      <c r="M1013" s="1"/>
+      <c r="N1013" s="2"/>
+      <c r="O1013" s="1"/>
+      <c r="P1013" s="1"/>
+      <c r="Q1013" s="1"/>
+      <c r="R1013" s="1"/>
+      <c r="S1013" s="1"/>
+      <c r="T1013" s="1"/>
+      <c r="U1013" s="1"/>
+      <c r="V1013" s="1"/>
+      <c r="W1013" s="1"/>
+      <c r="X1013" s="1"/>
+      <c r="Y1013" s="1"/>
+      <c r="Z1013" s="1"/>
+      <c r="AA1013" s="1"/>
+      <c r="AB1013" s="1"/>
+      <c r="AC1013" s="1"/>
+      <c r="AD1013" s="1"/>
+      <c r="AE1013" s="1"/>
+      <c r="AF1013" s="1"/>
+      <c r="AG1013" s="1"/>
+      <c r="AH1013" s="1"/>
+      <c r="AI1013" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A29:A38"/>
+    <mergeCell ref="A13:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38979,46 +39054,46 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="51" t="s">
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="49"/>
+      <c r="I6" s="52"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -39192,12 +39267,12 @@
     </row>
     <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
     </row>
@@ -68635,10 +68710,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C378BDBA-608F-43ED-BF6C-14DDA805CFD5}">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -68698,16 +68773,16 @@
         <v>201</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="T1" s="34" t="s">
         <v>195</v>
@@ -69138,7 +69213,7 @@
         <v>194</v>
       </c>
       <c r="T9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -69503,7 +69578,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>35</v>
+        <v>238</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>190</v>
@@ -69559,7 +69634,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>37</v>
+        <v>239</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>191</v>
@@ -69613,32 +69688,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19" s="25">
+        <v>0</v>
+      </c>
+      <c r="D19" s="25">
+        <v>1</v>
+      </c>
+      <c r="E19" s="25">
+        <v>1</v>
+      </c>
+      <c r="F19" s="25">
+        <v>0</v>
+      </c>
+      <c r="G19" s="25">
+        <v>0</v>
+      </c>
+      <c r="H19" s="25">
+        <v>0</v>
+      </c>
+      <c r="I19" s="25">
+        <v>0</v>
+      </c>
+      <c r="J19" s="25">
+        <v>0</v>
+      </c>
+      <c r="K19" s="25">
+        <v>0</v>
+      </c>
+      <c r="L19" s="25">
+        <v>0</v>
+      </c>
+      <c r="M19" s="25">
+        <v>1</v>
+      </c>
+      <c r="N19" s="25">
+        <v>0</v>
+      </c>
+      <c r="O19" s="25">
+        <v>0</v>
+      </c>
+      <c r="P19" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="25">
+        <v>0</v>
+      </c>
+      <c r="R19" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>198</v>
+        <v>240</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>191</v>
       </c>
       <c r="C20" s="25">
         <v>0</v>
@@ -69647,13 +69758,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="25">
         <v>0</v>
       </c>
       <c r="G20" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="25">
         <v>0</v>
@@ -69665,16 +69776,16 @@
         <v>0</v>
       </c>
       <c r="K20" s="25">
+        <v>0</v>
+      </c>
+      <c r="L20" s="25">
+        <v>0</v>
+      </c>
+      <c r="M20" s="25">
         <v>1</v>
       </c>
-      <c r="L20" s="25">
-        <v>1</v>
-      </c>
-      <c r="M20" s="25">
+      <c r="N20" s="25">
         <v>0</v>
-      </c>
-      <c r="N20" s="25">
-        <v>1</v>
       </c>
       <c r="O20" s="25">
         <v>0</v>
@@ -69686,90 +69797,50 @@
         <v>0</v>
       </c>
       <c r="R20" s="25">
-        <v>1</v>
-      </c>
-      <c r="S20" s="27" t="s">
-        <v>193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="C21" s="25">
-        <v>0</v>
-      </c>
-      <c r="D21" s="25">
-        <v>0</v>
-      </c>
-      <c r="E21" s="25">
-        <v>1</v>
-      </c>
-      <c r="F21" s="25">
-        <v>1</v>
-      </c>
-      <c r="G21" s="25">
-        <v>0</v>
-      </c>
-      <c r="H21" s="25">
-        <v>0</v>
-      </c>
-      <c r="I21" s="25">
-        <v>0</v>
-      </c>
-      <c r="J21" s="25">
-        <v>0</v>
-      </c>
-      <c r="K21" s="25">
-        <v>1</v>
-      </c>
-      <c r="L21" s="25">
-        <v>0</v>
-      </c>
-      <c r="M21" s="25">
-        <v>0</v>
-      </c>
-      <c r="N21" s="25">
-        <v>1</v>
-      </c>
-      <c r="O21" s="25">
-        <v>0</v>
-      </c>
-      <c r="P21" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="25">
-        <v>0</v>
-      </c>
-      <c r="R21" s="25">
-        <v>1</v>
-      </c>
-      <c r="S21" s="27"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>197</v>
+        <v>40</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>198</v>
       </c>
       <c r="C22" s="25">
         <v>0</v>
       </c>
       <c r="D22" s="25">
+        <v>1</v>
+      </c>
+      <c r="E22" s="25">
         <v>0</v>
       </c>
-      <c r="E22" s="25">
+      <c r="F22" s="25">
+        <v>0</v>
+      </c>
+      <c r="G22" s="25">
         <v>1</v>
-      </c>
-      <c r="F22" s="25">
-        <v>1</v>
-      </c>
-      <c r="G22" s="25">
-        <v>0</v>
       </c>
       <c r="H22" s="25">
         <v>0</v>
@@ -69781,16 +69852,16 @@
         <v>0</v>
       </c>
       <c r="K22" s="25">
+        <v>1</v>
+      </c>
+      <c r="L22" s="25">
+        <v>1</v>
+      </c>
+      <c r="M22" s="25">
         <v>0</v>
       </c>
-      <c r="L22" s="25">
-        <v>0</v>
-      </c>
-      <c r="M22" s="25">
+      <c r="N22" s="25">
         <v>1</v>
-      </c>
-      <c r="N22" s="25">
-        <v>0</v>
       </c>
       <c r="O22" s="25">
         <v>0</v>
@@ -69802,24 +69873,24 @@
         <v>0</v>
       </c>
       <c r="R22" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>197</v>
+        <v>42</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>181</v>
       </c>
       <c r="C23" s="25">
         <v>0</v>
       </c>
       <c r="D23" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="25">
         <v>1</v>
@@ -69840,7 +69911,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="25">
         <v>0</v>
@@ -69849,7 +69920,7 @@
         <v>0</v>
       </c>
       <c r="N23" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" s="25">
         <v>0</v>
@@ -69861,15 +69932,13 @@
         <v>0</v>
       </c>
       <c r="R23" s="25">
-        <v>0</v>
-      </c>
-      <c r="S23" s="27" t="s">
-        <v>194</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="S23" s="27"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B24" s="36" t="s">
         <v>197</v>
@@ -69878,16 +69947,16 @@
         <v>0</v>
       </c>
       <c r="D24" s="25">
+        <v>0</v>
+      </c>
+      <c r="E24" s="25">
         <v>1</v>
       </c>
-      <c r="E24" s="25">
+      <c r="F24" s="25">
+        <v>1</v>
+      </c>
+      <c r="G24" s="25">
         <v>0</v>
-      </c>
-      <c r="F24" s="25">
-        <v>0</v>
-      </c>
-      <c r="G24" s="25">
-        <v>1</v>
       </c>
       <c r="H24" s="25">
         <v>0</v>
@@ -69905,7 +69974,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="25">
         <v>0</v>
@@ -69927,34 +69996,73 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
+      <c r="A25" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="25">
+        <v>0</v>
+      </c>
+      <c r="J25" s="25">
+        <v>0</v>
+      </c>
+      <c r="K25" s="25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="25">
+        <v>0</v>
+      </c>
+      <c r="M25" s="25">
+        <v>0</v>
+      </c>
+      <c r="N25" s="25">
+        <v>0</v>
+      </c>
+      <c r="O25" s="25">
+        <v>0</v>
+      </c>
+      <c r="P25" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="25">
+        <v>0</v>
+      </c>
+      <c r="R25" s="25">
+        <v>0</v>
+      </c>
+      <c r="S25" s="27" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>198</v>
+        <v>46</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>197</v>
       </c>
       <c r="C26" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="25">
         <v>1</v>
@@ -69966,7 +70074,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="25">
         <v>0</v>
@@ -69998,75 +70106,36 @@
       <c r="Q26" s="25">
         <v>0</v>
       </c>
-      <c r="R26" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="S26" t="s">
-        <v>193</v>
+      <c r="R26" s="25">
+        <v>0</v>
+      </c>
+      <c r="S26" s="27" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="C27" s="25">
-        <v>1</v>
-      </c>
-      <c r="D27" s="25">
-        <v>1</v>
-      </c>
-      <c r="E27" s="25">
-        <v>0</v>
-      </c>
-      <c r="F27" s="25">
-        <v>0</v>
-      </c>
-      <c r="G27" s="25">
-        <v>0</v>
-      </c>
-      <c r="H27" s="25">
-        <v>0</v>
-      </c>
-      <c r="I27" s="25">
-        <v>0</v>
-      </c>
-      <c r="J27" s="25">
-        <v>0</v>
-      </c>
-      <c r="K27" s="25">
-        <v>0</v>
-      </c>
-      <c r="L27" s="25">
-        <v>0</v>
-      </c>
-      <c r="M27" s="25">
-        <v>0</v>
-      </c>
-      <c r="N27" s="25">
-        <v>0</v>
-      </c>
-      <c r="O27" s="25">
-        <v>0</v>
-      </c>
-      <c r="P27" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="25">
-        <v>0</v>
-      </c>
-      <c r="R27" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="S27" t="s">
-        <v>193</v>
-      </c>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>198</v>
@@ -70117,7 +70186,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="25" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="S28" t="s">
         <v>193</v>
@@ -70125,7 +70194,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>198</v>
@@ -70134,7 +70203,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="25">
         <v>0</v>
@@ -70176,24 +70245,24 @@
         <v>0</v>
       </c>
       <c r="R29" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="S29" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="S29" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>198</v>
       </c>
       <c r="C30" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="25">
         <v>0</v>
@@ -70232,24 +70301,24 @@
         <v>0</v>
       </c>
       <c r="Q30" s="25">
-        <v>1</v>
-      </c>
-      <c r="R30" s="25">
         <v>0</v>
       </c>
-      <c r="S30" s="24" t="s">
+      <c r="R30" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="S30" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="38" t="s">
-        <v>181</v>
+        <v>53</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>198</v>
       </c>
       <c r="C31" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="25">
         <v>0</v>
@@ -70288,21 +70357,24 @@
         <v>0</v>
       </c>
       <c r="P31" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="25">
         <v>0</v>
       </c>
-      <c r="R31" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R31" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="S31" s="24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
-        <v>238</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>181</v>
+        <v>55</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>198</v>
       </c>
       <c r="C32" s="25">
         <v>0</v>
@@ -70341,101 +70413,216 @@
         <v>0</v>
       </c>
       <c r="O32" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" s="25">
         <v>0</v>
       </c>
       <c r="Q32" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R32" s="25">
         <v>0</v>
       </c>
+      <c r="S32" s="24" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="26"/>
+      <c r="A33" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="25">
+        <v>0</v>
+      </c>
+      <c r="D33" s="25">
+        <v>0</v>
+      </c>
+      <c r="E33" s="25">
+        <v>0</v>
+      </c>
+      <c r="F33" s="25">
+        <v>0</v>
+      </c>
+      <c r="G33" s="25">
+        <v>0</v>
+      </c>
+      <c r="H33" s="25">
+        <v>0</v>
+      </c>
+      <c r="I33" s="25">
+        <v>0</v>
+      </c>
+      <c r="J33" s="25">
+        <v>0</v>
+      </c>
+      <c r="K33" s="25">
+        <v>0</v>
+      </c>
+      <c r="L33" s="25">
+        <v>0</v>
+      </c>
+      <c r="M33" s="25">
+        <v>0</v>
+      </c>
+      <c r="N33" s="25">
+        <v>0</v>
+      </c>
+      <c r="O33" s="25">
+        <v>0</v>
+      </c>
+      <c r="P33" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="25">
+        <v>0</v>
+      </c>
+      <c r="R33" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="C34" s="25">
+        <v>0</v>
+      </c>
+      <c r="D34" s="25">
+        <v>0</v>
+      </c>
+      <c r="E34" s="25">
+        <v>0</v>
+      </c>
+      <c r="F34" s="25">
+        <v>0</v>
+      </c>
+      <c r="G34" s="25">
+        <v>0</v>
+      </c>
+      <c r="H34" s="25">
+        <v>0</v>
+      </c>
+      <c r="I34" s="25">
+        <v>0</v>
+      </c>
+      <c r="J34" s="25">
+        <v>0</v>
+      </c>
+      <c r="K34" s="25">
+        <v>0</v>
+      </c>
+      <c r="L34" s="25">
+        <v>0</v>
+      </c>
+      <c r="M34" s="25">
+        <v>0</v>
+      </c>
+      <c r="N34" s="25">
+        <v>0</v>
+      </c>
+      <c r="O34" s="25">
+        <v>1</v>
+      </c>
+      <c r="P34" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="25">
+        <v>0</v>
+      </c>
+      <c r="R34" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="25"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="25"/>
+      <c r="O37" s="25"/>
+      <c r="P37" s="25"/>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="25"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="25"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="25"/>
+      <c r="Q38" s="25"/>
+      <c r="R38" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -70447,7 +70634,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -70558,7 +70745,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="B14" s="25">
         <v>1</v>
@@ -70566,7 +70753,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="B15" s="25">
         <v>1</v>
@@ -70577,7 +70764,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B16" s="25">
         <v>1</v>
@@ -70585,7 +70772,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B17" s="25">
         <v>1</v>
@@ -70593,7 +70780,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B18" s="25">
         <v>1</v>
@@ -70609,7 +70796,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B20" s="25">
         <v>1</v>
@@ -70617,7 +70804,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B21" s="25">
         <v>1</v>
@@ -70625,7 +70812,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B22" s="25">
         <v>1</v>
@@ -70633,7 +70820,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B23" s="25">
         <v>1</v>
@@ -70641,7 +70828,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B24" s="25">
         <v>1</v>
@@ -70649,7 +70836,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B25" s="25">
         <v>1</v>
@@ -70657,7 +70844,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B26" s="25">
         <v>1</v>
@@ -70665,7 +70852,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B27" s="25">
         <v>1</v>
@@ -70673,12 +70860,12 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integrate interrupt and rti
</commit_message>
<xml_diff>
--- a/Design/Processor Design Analysis.xlsx
+++ b/Design/Processor Design Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material\3rd CMP\First term\Computer arch\Project\MIPS-Microprocessor-Design\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849D829E-2972-4256-8039-F17F32458074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6C7A4F-98BE-48FB-8E6A-BD5E508AC1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="245">
   <si>
     <t>Category of Operations</t>
   </si>
@@ -758,6 +758,12 @@
   <si>
     <t>shr imm</t>
   </si>
+  <si>
+    <t>shl reg</t>
+  </si>
+  <si>
+    <t>shr reg</t>
+  </si>
 </sst>
 </file>
 
@@ -1294,8 +1300,8 @@
   </sheetPr>
   <dimension ref="A1:AI1013"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -70631,10 +70637,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04234B7-E967-4FCA-8035-6E4532CB5BC2}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -70862,10 +70868,32 @@
       <c r="A28" s="28" t="s">
         <v>229</v>
       </c>
+      <c r="B28" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>235</v>
+      </c>
+      <c r="B29" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B30" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B31" s="25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add jump immediate test case
</commit_message>
<xml_diff>
--- a/Design/Processor Design Analysis.xlsx
+++ b/Design/Processor Design Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material\3rd CMP\First term\Computer arch\Project\MIPS-Microprocessor-Design\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6C7A4F-98BE-48FB-8E6A-BD5E508AC1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBD4C06-9FC2-47DD-B119-4ABD3DBF46B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="246">
   <si>
     <t>Category of Operations</t>
   </si>
@@ -764,6 +764,9 @@
   <si>
     <t>shr reg</t>
   </si>
+  <si>
+    <t>jmpi</t>
+  </si>
 </sst>
 </file>
 
@@ -941,7 +944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -992,15 +995,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1014,7 +1014,6 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1023,9 +1022,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1042,7 +1038,6 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1053,17 +1048,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1300,8 +1287,8 @@
   </sheetPr>
   <dimension ref="A1:AI1013"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1313,7 +1300,7 @@
     <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="3.44140625" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="3.21875" style="30" customWidth="1"/>
+    <col min="8" max="8" width="3.21875" customWidth="1"/>
     <col min="10" max="10" width="3.21875" customWidth="1"/>
     <col min="12" max="12" width="3.6640625" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" customWidth="1"/>
@@ -1347,11 +1334,11 @@
         <v>3</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="36" t="s">
         <v>210</v>
       </c>
       <c r="J1" s="2"/>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="36" t="s">
         <v>211</v>
       </c>
       <c r="L1" s="2"/>
@@ -1421,7 +1408,7 @@
       <c r="AI2" s="3"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2"/>
@@ -1437,11 +1424,11 @@
         <v>9</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="4"/>
@@ -1472,7 +1459,7 @@
       <c r="AI3" s="3"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -1486,11 +1473,11 @@
         <v>14</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L4" s="4"/>
@@ -1521,7 +1508,7 @@
       <c r="AI4" s="3"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -1535,11 +1522,11 @@
         <v>16</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L5" s="4"/>
@@ -1573,7 +1560,7 @@
       <c r="AI6" s="3"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2"/>
@@ -1589,11 +1576,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="41" t="s">
+      <c r="K7" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L7" s="4"/>
@@ -1607,7 +1594,7 @@
       <c r="AI7" s="3"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
         <v>21</v>
@@ -1621,11 +1608,11 @@
         <v>14</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="41" t="s">
+      <c r="K8" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L8" s="4"/>
@@ -1639,7 +1626,7 @@
       <c r="AI8" s="3"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>22</v>
@@ -1653,11 +1640,11 @@
         <v>16</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L9" s="4"/>
@@ -1671,7 +1658,7 @@
       <c r="AI9" s="3"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>23</v>
@@ -1689,7 +1676,7 @@
         <v>11</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L10" s="4"/>
@@ -1703,7 +1690,7 @@
       <c r="AI10" s="3"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>25</v>
@@ -1721,7 +1708,7 @@
         <v>11</v>
       </c>
       <c r="J11" s="2"/>
-      <c r="K11" s="41" t="s">
+      <c r="K11" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="4"/>
@@ -1755,7 +1742,7 @@
       <c r="AI12" s="3"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="41" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="2"/>
@@ -1771,11 +1758,11 @@
         <v>9</v>
       </c>
       <c r="H13" s="9"/>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="9"/>
-      <c r="K13" s="41" t="s">
+      <c r="K13" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L13" s="4"/>
@@ -1789,7 +1776,7 @@
       <c r="AI13" s="3"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
         <v>31</v>
@@ -1803,11 +1790,11 @@
         <v>14</v>
       </c>
       <c r="H14" s="9"/>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J14" s="9"/>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="4"/>
@@ -1821,7 +1808,7 @@
       <c r="AI14" s="3"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1835,11 +1822,11 @@
         <v>16</v>
       </c>
       <c r="H15" s="9"/>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="9"/>
-      <c r="K15" s="41" t="s">
+      <c r="K15" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L15" s="4"/>
@@ -1853,7 +1840,7 @@
       <c r="AI15" s="3"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
         <v>33</v>
@@ -1867,11 +1854,11 @@
         <v>24</v>
       </c>
       <c r="H16" s="9"/>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="9"/>
-      <c r="K16" s="41" t="s">
+      <c r="K16" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L16" s="4"/>
@@ -1885,7 +1872,7 @@
       <c r="AI16" s="3"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
         <v>34</v>
@@ -1899,11 +1886,11 @@
         <v>26</v>
       </c>
       <c r="H17" s="9"/>
-      <c r="I17" s="41" t="s">
+      <c r="I17" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="9"/>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L17" s="4"/>
@@ -1917,7 +1904,7 @@
       <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
         <v>238</v>
@@ -1931,11 +1918,11 @@
         <v>36</v>
       </c>
       <c r="H18" s="9"/>
-      <c r="I18" s="41" t="s">
+      <c r="I18" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="9"/>
-      <c r="K18" s="41" t="s">
+      <c r="K18" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L18" s="4"/>
@@ -1949,7 +1936,7 @@
       <c r="AI18" s="3"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
         <v>239</v>
@@ -1963,11 +1950,11 @@
         <v>38</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="41" t="s">
+      <c r="I19" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="9"/>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L19" s="4"/>
@@ -1979,10 +1966,10 @@
       <c r="P19" s="2"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="4"/>
@@ -1994,26 +1981,26 @@
         <v>57</v>
       </c>
       <c r="H20" s="9"/>
-      <c r="I20" s="41" t="s">
+      <c r="I20" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="9"/>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="41" t="s">
+      <c r="M20" s="35" t="s">
         <v>44</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="O20" s="48"/>
+      <c r="O20" s="1"/>
       <c r="P20" s="2"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="4"/>
@@ -2025,19 +2012,19 @@
         <v>59</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="41" t="s">
+      <c r="I21" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="9"/>
-      <c r="K21" s="41" t="s">
+      <c r="K21" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L21" s="4"/>
-      <c r="M21" s="41" t="s">
+      <c r="M21" s="35" t="s">
         <v>44</v>
       </c>
       <c r="N21" s="2"/>
-      <c r="O21" s="48"/>
+      <c r="O21" s="1"/>
       <c r="P21" s="2"/>
       <c r="AI21" s="3"/>
     </row>
@@ -2063,7 +2050,7 @@
       <c r="AI22" s="3"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="41" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="2"/>
@@ -2079,11 +2066,11 @@
         <v>9</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="43" t="s">
+      <c r="I23" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J23" s="2"/>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L23" s="4"/>
@@ -2098,7 +2085,7 @@
       <c r="AI23" s="3"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
         <v>42</v>
@@ -2112,11 +2099,11 @@
         <v>14</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="43" t="s">
+      <c r="I24" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J24" s="2"/>
-      <c r="K24" s="41" t="s">
+      <c r="K24" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L24" s="4"/>
@@ -2131,7 +2118,7 @@
       <c r="AI24" s="3"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
         <v>43</v>
@@ -2145,11 +2132,11 @@
         <v>16</v>
       </c>
       <c r="H25" s="4"/>
-      <c r="I25" s="43" t="s">
+      <c r="I25" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J25" s="4"/>
-      <c r="K25" s="41" t="s">
+      <c r="K25" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L25" s="4"/>
@@ -2164,7 +2151,7 @@
       <c r="AI25" s="3"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="2"/>
       <c r="C26" s="1" t="s">
         <v>45</v>
@@ -2178,11 +2165,11 @@
         <v>24</v>
       </c>
       <c r="H26" s="9"/>
-      <c r="I26" s="41" t="s">
+      <c r="I26" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J26" s="9"/>
-      <c r="K26" s="41" t="s">
+      <c r="K26" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L26" s="4"/>
@@ -2197,7 +2184,7 @@
       <c r="AI26" s="3"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1" t="s">
         <v>46</v>
@@ -2211,11 +2198,11 @@
         <v>26</v>
       </c>
       <c r="H27" s="9"/>
-      <c r="I27" s="41" t="s">
+      <c r="I27" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J27" s="9"/>
-      <c r="K27" s="41" t="s">
+      <c r="K27" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L27" s="4"/>
@@ -2259,7 +2246,7 @@
       <c r="AI28" s="3"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="41" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="2"/>
@@ -2275,11 +2262,11 @@
         <v>9</v>
       </c>
       <c r="H29" s="2"/>
-      <c r="I29" s="43" t="s">
+      <c r="I29" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J29" s="2"/>
-      <c r="K29" s="41" t="s">
+      <c r="K29" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L29" s="4"/>
@@ -2298,7 +2285,7 @@
       <c r="AI29" s="3"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1" t="s">
         <v>50</v>
@@ -2312,11 +2299,11 @@
         <v>14</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="I30" s="43" t="s">
+      <c r="I30" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J30" s="2"/>
-      <c r="K30" s="41" t="s">
+      <c r="K30" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L30" s="4"/>
@@ -2335,7 +2322,7 @@
       <c r="AI30" s="3"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
         <v>51</v>
@@ -2349,11 +2336,11 @@
         <v>16</v>
       </c>
       <c r="H31" s="2"/>
-      <c r="I31" s="43" t="s">
+      <c r="I31" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J31" s="2"/>
-      <c r="K31" s="41" t="s">
+      <c r="K31" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L31" s="4"/>
@@ -2372,7 +2359,7 @@
       <c r="AI31" s="3"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="2"/>
       <c r="C32" s="12" t="s">
         <v>52</v>
@@ -2386,11 +2373,11 @@
         <v>24</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="43" t="s">
+      <c r="I32" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J32" s="2"/>
-      <c r="K32" s="41" t="s">
+      <c r="K32" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L32" s="4"/>
@@ -2409,7 +2396,7 @@
       <c r="AI32" s="3"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
         <v>53</v>
@@ -2423,11 +2410,11 @@
         <v>26</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="43" t="s">
+      <c r="I33" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J33" s="2"/>
-      <c r="K33" s="41" t="s">
+      <c r="K33" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L33" s="4"/>
@@ -2446,7 +2433,7 @@
       <c r="AI33" s="3"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="2"/>
       <c r="C34" s="12" t="s">
         <v>54</v>
@@ -2460,11 +2447,11 @@
         <v>36</v>
       </c>
       <c r="H34" s="2"/>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J34" s="2"/>
-      <c r="K34" s="43" t="s">
+      <c r="K34" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L34" s="4"/>
@@ -2487,7 +2474,7 @@
       <c r="AI34" s="3"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1" t="s">
         <v>55</v>
@@ -2501,11 +2488,11 @@
         <v>38</v>
       </c>
       <c r="H35" s="2"/>
-      <c r="I35" s="43" t="s">
+      <c r="I35" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J35" s="2"/>
-      <c r="K35" s="41" t="s">
+      <c r="K35" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L35" s="4"/>
@@ -2528,7 +2515,7 @@
       <c r="AI35" s="3"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="2"/>
       <c r="C36" s="12" t="s">
         <v>56</v>
@@ -2542,11 +2529,11 @@
         <v>57</v>
       </c>
       <c r="H36" s="2"/>
-      <c r="I36" s="41" t="s">
+      <c r="I36" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J36" s="2"/>
-      <c r="K36" s="43" t="s">
+      <c r="K36" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L36" s="4"/>
@@ -2569,7 +2556,7 @@
       <c r="AI36" s="3"/>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1" t="s">
         <v>58</v>
@@ -2583,11 +2570,11 @@
         <v>59</v>
       </c>
       <c r="H37" s="2"/>
-      <c r="I37" s="43" t="s">
+      <c r="I37" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J37" s="2"/>
-      <c r="K37" s="50" t="s">
+      <c r="K37" s="40" t="s">
         <v>11</v>
       </c>
       <c r="L37" s="4"/>
@@ -2610,7 +2597,7 @@
       <c r="AI37" s="3"/>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
+      <c r="A38" s="42"/>
       <c r="B38" s="2"/>
       <c r="C38" s="12" t="s">
         <v>60</v>
@@ -2628,7 +2615,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="2"/>
-      <c r="K38" s="41" t="s">
+      <c r="K38" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L38" s="2"/>
@@ -2650,9 +2637,9 @@
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
     </row>
-    <row r="39" spans="1:35" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
-      <c r="C39" s="47" t="s">
+      <c r="C39" s="39" t="s">
         <v>236</v>
       </c>
       <c r="D39" s="2"/>
@@ -2664,11 +2651,11 @@
         <v>237</v>
       </c>
       <c r="H39" s="2"/>
-      <c r="I39" s="43" t="s">
+      <c r="I39" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J39" s="2"/>
-      <c r="K39" s="50" t="s">
+      <c r="K39" s="40" t="s">
         <v>11</v>
       </c>
       <c r="L39" s="2"/>
@@ -2676,7 +2663,7 @@
         <v>12</v>
       </c>
       <c r="N39" s="2"/>
-      <c r="O39" s="45"/>
+      <c r="O39" s="1"/>
       <c r="P39" s="2"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
@@ -2749,7 +2736,7 @@
       <c r="AI41" s="3"/>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="41" t="s">
         <v>62</v>
       </c>
       <c r="B42" s="2"/>
@@ -2765,11 +2752,11 @@
         <v>10</v>
       </c>
       <c r="H42" s="2"/>
-      <c r="I42" s="43" t="s">
+      <c r="I42" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J42" s="2"/>
-      <c r="K42" s="43" t="s">
+      <c r="K42" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L42" s="4"/>
@@ -2794,7 +2781,7 @@
       <c r="AI42" s="3"/>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A43" s="52"/>
+      <c r="A43" s="42"/>
       <c r="B43" s="2"/>
       <c r="C43" s="1" t="s">
         <v>64</v>
@@ -2808,11 +2795,11 @@
         <v>10</v>
       </c>
       <c r="H43" s="2"/>
-      <c r="I43" s="43" t="s">
+      <c r="I43" s="37" t="s">
         <v>10</v>
       </c>
       <c r="J43" s="2"/>
-      <c r="K43" s="43" t="s">
+      <c r="K43" s="37" t="s">
         <v>11</v>
       </c>
       <c r="L43" s="4"/>
@@ -38798,7 +38785,7 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>146</v>
       </c>
       <c r="E4" s="16" t="s">
@@ -38812,7 +38799,7 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>147</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -38826,7 +38813,7 @@
       <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>148</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -38840,7 +38827,7 @@
       <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>149</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -38854,7 +38841,7 @@
       <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>150</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -38868,7 +38855,7 @@
       <c r="C9" s="3">
         <v>5</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>151</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -38882,7 +38869,7 @@
       <c r="C10" s="3">
         <v>6</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>152</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -38896,7 +38883,7 @@
       <c r="C11" s="3">
         <v>7</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>153</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -38910,7 +38897,7 @@
       <c r="C12" s="3">
         <v>8</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>154</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -38924,7 +38911,7 @@
       <c r="C13" s="3">
         <v>9</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>155</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -38938,7 +38925,7 @@
       <c r="C14" s="3">
         <v>10</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>156</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -38952,7 +38939,7 @@
       <c r="C15" s="3">
         <v>11</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>157</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -38966,7 +38953,7 @@
       <c r="C16" s="3">
         <v>12</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>158</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -38980,7 +38967,7 @@
       <c r="C17" s="3">
         <v>13</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="21" t="s">
         <v>159</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -39060,46 +39047,46 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="54" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="52"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -39273,12 +39260,12 @@
     </row>
     <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
     </row>
@@ -39430,7 +39417,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" s="20" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
@@ -39442,7 +39429,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" s="20" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
@@ -39508,23 +39495,23 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="25"/>
+      <c r="D26" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -68729,493 +68716,491 @@
     <col min="4" max="5" width="13.88671875" customWidth="1"/>
     <col min="11" max="11" width="14.44140625" customWidth="1"/>
     <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="16.44140625" customWidth="1"/>
-    <col min="14" max="17" width="16.44140625" style="46" customWidth="1"/>
-    <col min="18" max="18" width="16.44140625" style="40" customWidth="1"/>
+    <col min="13" max="18" width="16.44140625" customWidth="1"/>
     <col min="19" max="19" width="17.77734375" customWidth="1"/>
     <col min="20" max="20" width="37.6640625" customWidth="1"/>
     <col min="21" max="21" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="30" t="s">
         <v>230</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="U1" s="27" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="22">
         <v>0</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="22">
         <v>0</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="22">
         <v>0</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="22">
         <v>0</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="22">
         <v>0</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="22">
         <v>0</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="22">
         <v>0</v>
       </c>
-      <c r="J2" s="25">
+      <c r="J2" s="22">
         <v>0</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="22">
         <v>0</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="22">
         <v>0</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="22">
         <v>0</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="22">
         <v>0</v>
       </c>
-      <c r="O2" s="25">
+      <c r="O2" s="22">
         <v>0</v>
       </c>
-      <c r="P2" s="25">
+      <c r="P2" s="22">
         <v>0</v>
       </c>
-      <c r="Q2" s="25">
+      <c r="Q2" s="22">
         <v>0</v>
       </c>
-      <c r="R2" s="25">
+      <c r="R2" s="22">
         <v>0</v>
       </c>
-      <c r="T2" s="35" t="s">
+      <c r="T2" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="U2" s="39" t="s">
+      <c r="U2" s="34" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="22">
         <v>0</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="22">
         <v>0</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="22">
         <v>0</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="22">
         <v>0</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="22">
         <v>0</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="22">
         <v>0</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="22">
         <v>0</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="22">
         <v>0</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="22">
         <v>0</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="22">
         <v>0</v>
       </c>
-      <c r="M3" s="25">
+      <c r="M3" s="22">
         <v>0</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3" s="22">
         <v>0</v>
       </c>
-      <c r="O3" s="25">
+      <c r="O3" s="22">
         <v>0</v>
       </c>
-      <c r="P3" s="25">
+      <c r="P3" s="22">
         <v>0</v>
       </c>
-      <c r="Q3" s="25">
+      <c r="Q3" s="22">
         <v>0</v>
       </c>
-      <c r="R3" s="25">
+      <c r="R3" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="22">
         <v>0</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <v>0</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="22">
         <v>0</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="22">
         <v>0</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="22">
         <v>0</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="22">
         <v>0</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="22">
         <v>0</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="22">
         <v>0</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="22">
         <v>0</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="22">
         <v>0</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="22">
         <v>0</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="22">
         <v>0</v>
       </c>
-      <c r="O4" s="25">
+      <c r="O4" s="22">
         <v>0</v>
       </c>
-      <c r="P4" s="25">
+      <c r="P4" s="22">
         <v>0</v>
       </c>
-      <c r="Q4" s="25">
+      <c r="Q4" s="22">
         <v>0</v>
       </c>
-      <c r="R4" s="25">
+      <c r="R4" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="22">
         <v>0</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <v>1</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <v>1</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>0</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <v>0</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <v>0</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="22">
         <v>0</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="22">
         <v>0</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="22">
         <v>0</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="22">
         <v>0</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="22">
         <v>0</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="22">
         <v>0</v>
       </c>
-      <c r="O6" s="25">
+      <c r="O6" s="22">
         <v>0</v>
       </c>
-      <c r="P6" s="25">
+      <c r="P6" s="22">
         <v>0</v>
       </c>
-      <c r="Q6" s="25">
+      <c r="Q6" s="22">
         <v>0</v>
       </c>
-      <c r="R6" s="25">
+      <c r="R6" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="22">
         <v>0</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="22">
         <v>1</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <v>1</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="22">
         <v>0</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="22">
         <v>0</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="22">
         <v>0</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="22">
         <v>0</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="22">
         <v>0</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="22">
         <v>0</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="22">
         <v>0</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="22">
         <v>0</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="22">
         <v>0</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="22">
         <v>0</v>
       </c>
-      <c r="P7" s="25">
+      <c r="P7" s="22">
         <v>0</v>
       </c>
-      <c r="Q7" s="25">
+      <c r="Q7" s="22">
         <v>0</v>
       </c>
-      <c r="R7" s="25">
+      <c r="R7" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="22">
         <v>0</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="22">
         <v>1</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="22">
         <v>1</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>0</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="22">
         <v>0</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="22">
         <v>0</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="22">
         <v>0</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="22">
         <v>0</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="22">
         <v>0</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="22">
         <v>0</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="22">
         <v>0</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="22">
         <v>0</v>
       </c>
-      <c r="O8" s="25">
+      <c r="O8" s="22">
         <v>0</v>
       </c>
-      <c r="P8" s="25">
+      <c r="P8" s="22">
         <v>0</v>
       </c>
-      <c r="Q8" s="25">
+      <c r="Q8" s="22">
         <v>0</v>
       </c>
-      <c r="R8" s="25">
+      <c r="R8" s="22">
         <v>0</v>
       </c>
-      <c r="S8" s="27"/>
+      <c r="S8" s="24"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="22">
         <v>0</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="22">
         <v>1</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <v>0</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="22">
         <v>0</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="22">
         <v>0</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="22">
         <v>1</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="22">
         <v>1</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="22">
         <v>0</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="22">
         <v>0</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="22">
         <v>0</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="22">
         <v>0</v>
       </c>
-      <c r="N9" s="25">
+      <c r="N9" s="22">
         <v>0</v>
       </c>
-      <c r="O9" s="25">
+      <c r="O9" s="22">
         <v>0</v>
       </c>
-      <c r="P9" s="25">
+      <c r="P9" s="22">
         <v>0</v>
       </c>
-      <c r="Q9" s="25">
+      <c r="Q9" s="22">
         <v>0</v>
       </c>
-      <c r="R9" s="25">
+      <c r="R9" s="22">
         <v>0</v>
       </c>
-      <c r="S9" s="44" t="s">
+      <c r="S9" s="38" t="s">
         <v>194</v>
       </c>
       <c r="T9" t="s">
@@ -69223,975 +69208,975 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="22">
         <v>0</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <v>0</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
         <v>1</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="22">
         <v>0</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="22">
         <v>0</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="22">
         <v>1</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="22">
         <v>0</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="22">
         <v>1</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="22">
         <v>0</v>
       </c>
-      <c r="L10" s="25">
+      <c r="L10" s="22">
         <v>0</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="22">
         <v>0</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="22">
         <v>0</v>
       </c>
-      <c r="O10" s="25">
+      <c r="O10" s="22">
         <v>0</v>
       </c>
-      <c r="P10" s="25">
+      <c r="P10" s="22">
         <v>0</v>
       </c>
-      <c r="Q10" s="25">
+      <c r="Q10" s="22">
         <v>0</v>
       </c>
-      <c r="R10" s="25">
+      <c r="R10" s="22">
         <v>0</v>
       </c>
-      <c r="S10" s="27"/>
+      <c r="S10" s="24"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="22">
         <v>0</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="22">
         <v>1</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="22">
         <v>1</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="22">
         <v>0</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="22">
         <v>0</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="22">
         <v>0</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="22">
         <v>0</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="22">
         <v>0</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="22">
         <v>0</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="22">
         <v>0</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="22">
         <v>0</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12" s="22">
         <v>0</v>
       </c>
-      <c r="O12" s="25">
+      <c r="O12" s="22">
         <v>0</v>
       </c>
-      <c r="P12" s="25">
+      <c r="P12" s="22">
         <v>0</v>
       </c>
-      <c r="Q12" s="25">
+      <c r="Q12" s="22">
         <v>0</v>
       </c>
-      <c r="R12" s="25">
+      <c r="R12" s="22">
         <v>0</v>
       </c>
-      <c r="S12" s="27" t="s">
+      <c r="S12" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="22">
         <v>0</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="22">
         <v>1</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="22">
         <v>1</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="22">
         <v>0</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="22">
         <v>0</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="22">
         <v>0</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="22">
         <v>0</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13" s="22">
         <v>0</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="22">
         <v>0</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="22">
         <v>0</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="22">
         <v>0</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="22">
         <v>0</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="22">
         <v>0</v>
       </c>
-      <c r="P13" s="25">
+      <c r="P13" s="22">
         <v>0</v>
       </c>
-      <c r="Q13" s="25">
+      <c r="Q13" s="22">
         <v>0</v>
       </c>
-      <c r="R13" s="25">
+      <c r="R13" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="22">
         <v>0</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <v>1</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
         <v>1</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="22">
         <v>0</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="22">
         <v>0</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="22">
         <v>0</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="22">
         <v>0</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="22">
         <v>0</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="22">
         <v>0</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="22">
         <v>0</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="22">
         <v>0</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="22">
         <v>0</v>
       </c>
-      <c r="O14" s="25">
+      <c r="O14" s="22">
         <v>0</v>
       </c>
-      <c r="P14" s="25">
+      <c r="P14" s="22">
         <v>0</v>
       </c>
-      <c r="Q14" s="25">
+      <c r="Q14" s="22">
         <v>0</v>
       </c>
-      <c r="R14" s="25">
+      <c r="R14" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="22">
         <v>0</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="22">
         <v>1</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="22">
         <v>1</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="22">
         <v>0</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="22">
         <v>0</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="22">
         <v>0</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="22">
         <v>0</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="22">
         <v>0</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="22">
         <v>0</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15" s="22">
         <v>0</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="22">
         <v>0</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="22">
         <v>0</v>
       </c>
-      <c r="O15" s="25">
+      <c r="O15" s="22">
         <v>0</v>
       </c>
-      <c r="P15" s="25">
+      <c r="P15" s="22">
         <v>0</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q15" s="22">
         <v>0</v>
       </c>
-      <c r="R15" s="25">
+      <c r="R15" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="22">
         <v>0</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="22">
         <v>1</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
         <v>1</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="22">
         <v>0</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="22">
         <v>0</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="22">
         <v>0</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="22">
         <v>0</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="22">
         <v>0</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="22">
         <v>0</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="22">
         <v>0</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="22">
         <v>0</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="22">
         <v>0</v>
       </c>
-      <c r="O16" s="25">
+      <c r="O16" s="22">
         <v>0</v>
       </c>
-      <c r="P16" s="25">
+      <c r="P16" s="22">
         <v>0</v>
       </c>
-      <c r="Q16" s="25">
+      <c r="Q16" s="22">
         <v>0</v>
       </c>
-      <c r="R16" s="25">
+      <c r="R16" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="22">
         <v>0</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="22">
         <v>1</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="22">
         <v>1</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="22">
         <v>0</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="22">
         <v>0</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="22">
         <v>0</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="22">
         <v>0</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="22">
         <v>0</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="22">
         <v>0</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="22">
         <v>0</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="22">
         <v>0</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="22">
         <v>0</v>
       </c>
-      <c r="O17" s="25">
+      <c r="O17" s="22">
         <v>0</v>
       </c>
-      <c r="P17" s="25">
+      <c r="P17" s="22">
         <v>0</v>
       </c>
-      <c r="Q17" s="25">
+      <c r="Q17" s="22">
         <v>0</v>
       </c>
-      <c r="R17" s="25">
+      <c r="R17" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="22">
         <v>0</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="22">
         <v>1</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
         <v>1</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="22">
         <v>0</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="22">
         <v>0</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="22">
         <v>0</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="22">
         <v>0</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="22">
         <v>0</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="22">
         <v>0</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="22">
         <v>0</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="22">
         <v>0</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="22">
         <v>0</v>
       </c>
-      <c r="O18" s="25">
+      <c r="O18" s="22">
         <v>0</v>
       </c>
-      <c r="P18" s="25">
+      <c r="P18" s="22">
         <v>0</v>
       </c>
-      <c r="Q18" s="25">
+      <c r="Q18" s="22">
         <v>0</v>
       </c>
-      <c r="R18" s="25">
+      <c r="R18" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="22">
         <v>0</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="22">
         <v>1</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="22">
         <v>1</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="22">
         <v>0</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="22">
         <v>0</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="22">
         <v>0</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="22">
         <v>0</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="22">
         <v>0</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="22">
         <v>0</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="22">
         <v>0</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="22">
         <v>1</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="22">
         <v>0</v>
       </c>
-      <c r="O19" s="25">
+      <c r="O19" s="22">
         <v>0</v>
       </c>
-      <c r="P19" s="25">
+      <c r="P19" s="22">
         <v>0</v>
       </c>
-      <c r="Q19" s="25">
+      <c r="Q19" s="22">
         <v>0</v>
       </c>
-      <c r="R19" s="25">
+      <c r="R19" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="22">
         <v>0</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <v>1</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="22">
         <v>1</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="22">
         <v>0</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="22">
         <v>0</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="22">
         <v>0</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="22">
         <v>0</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20" s="22">
         <v>0</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="22">
         <v>0</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20" s="22">
         <v>0</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="22">
         <v>1</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20" s="22">
         <v>0</v>
       </c>
-      <c r="O20" s="25">
+      <c r="O20" s="22">
         <v>0</v>
       </c>
-      <c r="P20" s="25">
+      <c r="P20" s="22">
         <v>0</v>
       </c>
-      <c r="Q20" s="25">
+      <c r="Q20" s="22">
         <v>0</v>
       </c>
-      <c r="R20" s="25">
+      <c r="R20" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="22">
         <v>0</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="22">
         <v>1</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="22">
         <v>0</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="22">
         <v>0</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="22">
         <v>1</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="22">
         <v>0</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="22">
         <v>0</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22" s="22">
         <v>0</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22" s="22">
         <v>1</v>
       </c>
-      <c r="L22" s="25">
+      <c r="L22" s="22">
         <v>1</v>
       </c>
-      <c r="M22" s="25">
+      <c r="M22" s="22">
         <v>0</v>
       </c>
-      <c r="N22" s="25">
+      <c r="N22" s="22">
         <v>1</v>
       </c>
-      <c r="O22" s="25">
+      <c r="O22" s="22">
         <v>0</v>
       </c>
-      <c r="P22" s="25">
+      <c r="P22" s="22">
         <v>0</v>
       </c>
-      <c r="Q22" s="25">
+      <c r="Q22" s="22">
         <v>0</v>
       </c>
-      <c r="R22" s="25">
+      <c r="R22" s="22">
         <v>1</v>
       </c>
-      <c r="S22" s="27" t="s">
+      <c r="S22" s="24" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23" s="22">
         <v>0</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="22">
         <v>0</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="22">
         <v>1</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="22">
         <v>1</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="22">
         <v>0</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="22">
         <v>0</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I23" s="22">
         <v>0</v>
       </c>
-      <c r="J23" s="25">
+      <c r="J23" s="22">
         <v>0</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="22">
         <v>1</v>
       </c>
-      <c r="L23" s="25">
+      <c r="L23" s="22">
         <v>0</v>
       </c>
-      <c r="M23" s="25">
+      <c r="M23" s="22">
         <v>0</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N23" s="22">
         <v>1</v>
       </c>
-      <c r="O23" s="25">
+      <c r="O23" s="22">
         <v>0</v>
       </c>
-      <c r="P23" s="25">
+      <c r="P23" s="22">
         <v>0</v>
       </c>
-      <c r="Q23" s="25">
+      <c r="Q23" s="22">
         <v>0</v>
       </c>
-      <c r="R23" s="25">
+      <c r="R23" s="22">
         <v>1</v>
       </c>
-      <c r="S23" s="27"/>
+      <c r="S23" s="24"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="22">
         <v>0</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <v>0</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="22">
         <v>1</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="22">
         <v>1</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="22">
         <v>0</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="22">
         <v>0</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24" s="22">
         <v>0</v>
       </c>
-      <c r="J24" s="25">
+      <c r="J24" s="22">
         <v>0</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="22">
         <v>0</v>
       </c>
-      <c r="L24" s="25">
+      <c r="L24" s="22">
         <v>0</v>
       </c>
-      <c r="M24" s="25">
+      <c r="M24" s="22">
         <v>1</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="22">
         <v>0</v>
       </c>
-      <c r="O24" s="25">
+      <c r="O24" s="22">
         <v>0</v>
       </c>
-      <c r="P24" s="25">
+      <c r="P24" s="22">
         <v>0</v>
       </c>
-      <c r="Q24" s="25">
+      <c r="Q24" s="22">
         <v>0</v>
       </c>
-      <c r="R24" s="25">
+      <c r="R24" s="22">
         <v>0</v>
       </c>
-      <c r="S24" s="27" t="s">
+      <c r="S24" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="22">
         <v>0</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="22">
         <v>1</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="22">
         <v>1</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="22">
         <v>1</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="22">
         <v>0</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="22">
         <v>0</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="22">
         <v>0</v>
       </c>
-      <c r="J25" s="25">
+      <c r="J25" s="22">
         <v>0</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25" s="22">
         <v>0</v>
       </c>
-      <c r="L25" s="25">
+      <c r="L25" s="22">
         <v>0</v>
       </c>
-      <c r="M25" s="25">
+      <c r="M25" s="22">
         <v>0</v>
       </c>
-      <c r="N25" s="25">
+      <c r="N25" s="22">
         <v>0</v>
       </c>
-      <c r="O25" s="25">
+      <c r="O25" s="22">
         <v>0</v>
       </c>
-      <c r="P25" s="25">
+      <c r="P25" s="22">
         <v>0</v>
       </c>
-      <c r="Q25" s="25">
+      <c r="Q25" s="22">
         <v>0</v>
       </c>
-      <c r="R25" s="25">
+      <c r="R25" s="22">
         <v>0</v>
       </c>
-      <c r="S25" s="27" t="s">
+      <c r="S25" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="22">
         <v>0</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="22">
         <v>1</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="22">
         <v>0</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="22">
         <v>0</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="22">
         <v>1</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="22">
         <v>0</v>
       </c>
-      <c r="I26" s="25">
+      <c r="I26" s="22">
         <v>0</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26" s="22">
         <v>0</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="22">
         <v>0</v>
       </c>
-      <c r="L26" s="25">
+      <c r="L26" s="22">
         <v>0</v>
       </c>
-      <c r="M26" s="25">
+      <c r="M26" s="22">
         <v>0</v>
       </c>
-      <c r="N26" s="25">
+      <c r="N26" s="22">
         <v>0</v>
       </c>
-      <c r="O26" s="25">
+      <c r="O26" s="22">
         <v>0</v>
       </c>
-      <c r="P26" s="25">
+      <c r="P26" s="22">
         <v>0</v>
       </c>
-      <c r="Q26" s="25">
+      <c r="Q26" s="22">
         <v>0</v>
       </c>
-      <c r="R26" s="25">
+      <c r="R26" s="22">
         <v>0</v>
       </c>
-      <c r="S26" s="27" t="s">
+      <c r="S26" s="24" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="22">
         <v>1</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="22">
         <v>1</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="22">
         <v>0</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="22">
         <v>0</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="22">
         <v>0</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H28" s="22">
         <v>0</v>
       </c>
-      <c r="I28" s="25">
+      <c r="I28" s="22">
         <v>0</v>
       </c>
-      <c r="J28" s="25">
+      <c r="J28" s="22">
         <v>0</v>
       </c>
-      <c r="K28" s="25">
+      <c r="K28" s="22">
         <v>0</v>
       </c>
-      <c r="L28" s="25">
+      <c r="L28" s="22">
         <v>0</v>
       </c>
-      <c r="M28" s="25">
+      <c r="M28" s="22">
         <v>0</v>
       </c>
-      <c r="N28" s="25">
+      <c r="N28" s="22">
         <v>0</v>
       </c>
-      <c r="O28" s="25">
+      <c r="O28" s="22">
         <v>0</v>
       </c>
-      <c r="P28" s="25">
+      <c r="P28" s="22">
         <v>0</v>
       </c>
-      <c r="Q28" s="25">
+      <c r="Q28" s="22">
         <v>0</v>
       </c>
-      <c r="R28" s="25" t="s">
+      <c r="R28" s="22" t="s">
         <v>231</v>
       </c>
       <c r="S28" t="s">
@@ -70199,58 +70184,58 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="22">
         <v>1</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="22">
         <v>1</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="22">
         <v>0</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="22">
         <v>0</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="22">
         <v>0</v>
       </c>
-      <c r="H29" s="25">
+      <c r="H29" s="22">
         <v>0</v>
       </c>
-      <c r="I29" s="25">
+      <c r="I29" s="22">
         <v>0</v>
       </c>
-      <c r="J29" s="25">
+      <c r="J29" s="22">
         <v>0</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="22">
         <v>0</v>
       </c>
-      <c r="L29" s="25">
+      <c r="L29" s="22">
         <v>0</v>
       </c>
-      <c r="M29" s="25">
+      <c r="M29" s="22">
         <v>0</v>
       </c>
-      <c r="N29" s="25">
+      <c r="N29" s="22">
         <v>0</v>
       </c>
-      <c r="O29" s="25">
+      <c r="O29" s="22">
         <v>0</v>
       </c>
-      <c r="P29" s="25">
+      <c r="P29" s="22">
         <v>0</v>
       </c>
-      <c r="Q29" s="25">
+      <c r="Q29" s="22">
         <v>0</v>
       </c>
-      <c r="R29" s="25" t="s">
+      <c r="R29" s="22" t="s">
         <v>232</v>
       </c>
       <c r="S29" t="s">
@@ -70258,58 +70243,58 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C30" s="25">
+      <c r="C30" s="22">
         <v>1</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="22">
         <v>1</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="22">
         <v>0</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="22">
         <v>0</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="22">
         <v>0</v>
       </c>
-      <c r="H30" s="25">
+      <c r="H30" s="22">
         <v>0</v>
       </c>
-      <c r="I30" s="25">
+      <c r="I30" s="22">
         <v>0</v>
       </c>
-      <c r="J30" s="25">
+      <c r="J30" s="22">
         <v>0</v>
       </c>
-      <c r="K30" s="25">
+      <c r="K30" s="22">
         <v>0</v>
       </c>
-      <c r="L30" s="25">
+      <c r="L30" s="22">
         <v>0</v>
       </c>
-      <c r="M30" s="25">
+      <c r="M30" s="22">
         <v>0</v>
       </c>
-      <c r="N30" s="25">
+      <c r="N30" s="22">
         <v>0</v>
       </c>
-      <c r="O30" s="25">
+      <c r="O30" s="22">
         <v>0</v>
       </c>
-      <c r="P30" s="25">
+      <c r="P30" s="22">
         <v>0</v>
       </c>
-      <c r="Q30" s="25">
+      <c r="Q30" s="22">
         <v>0</v>
       </c>
-      <c r="R30" s="25" t="s">
+      <c r="R30" s="22" t="s">
         <v>233</v>
       </c>
       <c r="S30" t="s">
@@ -70317,318 +70302,318 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="22">
         <v>1</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="22">
         <v>0</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="22">
         <v>0</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="22">
         <v>0</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="22">
         <v>0</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="22">
         <v>0</v>
       </c>
-      <c r="I31" s="25">
+      <c r="I31" s="22">
         <v>0</v>
       </c>
-      <c r="J31" s="25">
+      <c r="J31" s="22">
         <v>0</v>
       </c>
-      <c r="K31" s="25">
+      <c r="K31" s="22">
         <v>0</v>
       </c>
-      <c r="L31" s="25">
+      <c r="L31" s="22">
         <v>0</v>
       </c>
-      <c r="M31" s="25">
+      <c r="M31" s="22">
         <v>0</v>
       </c>
-      <c r="N31" s="25">
+      <c r="N31" s="22">
         <v>0</v>
       </c>
-      <c r="O31" s="25">
+      <c r="O31" s="22">
         <v>0</v>
       </c>
-      <c r="P31" s="25">
+      <c r="P31" s="22">
         <v>0</v>
       </c>
-      <c r="Q31" s="25">
+      <c r="Q31" s="22">
         <v>0</v>
       </c>
-      <c r="R31" s="25" t="s">
+      <c r="R31" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="S31" s="24" t="s">
+      <c r="S31" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C32" s="25">
+      <c r="C32" s="22">
         <v>0</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="22">
         <v>0</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="22">
         <v>0</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="22">
         <v>0</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="22">
         <v>0</v>
       </c>
-      <c r="H32" s="25">
+      <c r="H32" s="22">
         <v>0</v>
       </c>
-      <c r="I32" s="25">
+      <c r="I32" s="22">
         <v>0</v>
       </c>
-      <c r="J32" s="25">
+      <c r="J32" s="22">
         <v>0</v>
       </c>
-      <c r="K32" s="25">
+      <c r="K32" s="22">
         <v>0</v>
       </c>
-      <c r="L32" s="25">
+      <c r="L32" s="22">
         <v>0</v>
       </c>
-      <c r="M32" s="25">
+      <c r="M32" s="22">
         <v>0</v>
       </c>
-      <c r="N32" s="25">
+      <c r="N32" s="22">
         <v>0</v>
       </c>
-      <c r="O32" s="25">
+      <c r="O32" s="22">
         <v>0</v>
       </c>
-      <c r="P32" s="25">
+      <c r="P32" s="22">
         <v>0</v>
       </c>
-      <c r="Q32" s="25">
+      <c r="Q32" s="22">
         <v>1</v>
       </c>
-      <c r="R32" s="25">
+      <c r="R32" s="22">
         <v>0</v>
       </c>
-      <c r="S32" s="24" t="s">
+      <c r="S32" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C33" s="25">
+      <c r="C33" s="22">
         <v>0</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="22">
         <v>0</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="22">
         <v>0</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="22">
         <v>0</v>
       </c>
-      <c r="G33" s="25">
+      <c r="G33" s="22">
         <v>0</v>
       </c>
-      <c r="H33" s="25">
+      <c r="H33" s="22">
         <v>0</v>
       </c>
-      <c r="I33" s="25">
+      <c r="I33" s="22">
         <v>0</v>
       </c>
-      <c r="J33" s="25">
+      <c r="J33" s="22">
         <v>0</v>
       </c>
-      <c r="K33" s="25">
+      <c r="K33" s="22">
         <v>0</v>
       </c>
-      <c r="L33" s="25">
+      <c r="L33" s="22">
         <v>0</v>
       </c>
-      <c r="M33" s="25">
+      <c r="M33" s="22">
         <v>0</v>
       </c>
-      <c r="N33" s="25">
+      <c r="N33" s="22">
         <v>0</v>
       </c>
-      <c r="O33" s="25">
+      <c r="O33" s="22">
         <v>0</v>
       </c>
-      <c r="P33" s="25">
+      <c r="P33" s="22">
         <v>1</v>
       </c>
-      <c r="Q33" s="25">
+      <c r="Q33" s="22">
         <v>0</v>
       </c>
-      <c r="R33" s="25">
+      <c r="R33" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="22">
         <v>0</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="22">
         <v>0</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="22">
         <v>0</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="22">
         <v>0</v>
       </c>
-      <c r="G34" s="25">
+      <c r="G34" s="22">
         <v>0</v>
       </c>
-      <c r="H34" s="25">
+      <c r="H34" s="22">
         <v>0</v>
       </c>
-      <c r="I34" s="25">
+      <c r="I34" s="22">
         <v>0</v>
       </c>
-      <c r="J34" s="25">
+      <c r="J34" s="22">
         <v>0</v>
       </c>
-      <c r="K34" s="25">
+      <c r="K34" s="22">
         <v>0</v>
       </c>
-      <c r="L34" s="25">
+      <c r="L34" s="22">
         <v>0</v>
       </c>
-      <c r="M34" s="25">
+      <c r="M34" s="22">
         <v>0</v>
       </c>
-      <c r="N34" s="25">
+      <c r="N34" s="22">
         <v>0</v>
       </c>
-      <c r="O34" s="25">
+      <c r="O34" s="22">
         <v>1</v>
       </c>
-      <c r="P34" s="25">
+      <c r="P34" s="22">
         <v>0</v>
       </c>
-      <c r="Q34" s="25">
+      <c r="Q34" s="22">
         <v>0</v>
       </c>
-      <c r="R34" s="25">
+      <c r="R34" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
-      <c r="Q35" s="26"/>
-      <c r="R35" s="26"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="26"/>
-      <c r="Q36" s="26"/>
-      <c r="R36" s="26"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="25"/>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="25"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="25"/>
-      <c r="P38" s="25"/>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="25"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -70637,262 +70622,270 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04234B7-E967-4FCA-8035-6E4532CB5BC2}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="22">
         <v>1</v>
       </c>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="B26" s="25">
+      <c r="B26" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="B32" s="22">
         <v>1</v>
       </c>
     </row>

</xml_diff>